<commit_message>
Fixed bg errors to be sqrt(sum_w2)
</commit_message>
<xml_diff>
--- a/data/plotting_lut.xlsx
+++ b/data/plotting_lut.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="datasets" sheetId="1" state="visible" r:id="rId2"/>
@@ -359,7 +359,7 @@
     <t xml:space="preserve">jet</t>
   </si>
   <si>
-    <t xml:space="preserve">n_jets &gt; 0</t>
+    <t xml:space="preserve">n_jets &gt; 0 or n_fwdjets &gt; 0</t>
   </si>
   <si>
     <t xml:space="preserve">jet_phi</t>
@@ -425,7 +425,7 @@
     <t xml:space="preserve">Entries \,/\, 20 \, GeV</t>
   </si>
   <si>
-    <t xml:space="preserve">n_bjets &gt; 0 and n_jets &gt; 0</t>
+    <t xml:space="preserve">n_bjets &gt; 0 and (n_jets &gt; 0 or n_fwdjets &gt; 0)</t>
   </si>
   <si>
     <t xml:space="preserve">dijet_phi</t>
@@ -693,7 +693,7 @@
   </sheetPr>
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
@@ -701,12 +701,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.3826530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.4744897959184"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.5918367346939"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1275510204082"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.5765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.67857142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.7908163265306"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.4030612244898"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -1228,10 +1228,10 @@
   </sheetPr>
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H40" activeCellId="0" sqref="H40"/>
+      <selection pane="bottomLeft" activeCell="C35" activeCellId="0" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1239,10 +1239,10 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9387755102041"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.2040816326531"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.2602040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.3061224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.4795918367347"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.4489795918367"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -2070,13 +2070,13 @@
         <v>137</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>-2.4</v>
+        <v>-5</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>2.4</v>
+        <v>5</v>
       </c>
       <c r="E34" s="0" t="s">
         <v>138</v>

</xml_diff>

<commit_message>
Implemented parameter varying (might need tweaking) and 2D fitting
</commit_message>
<xml_diff>
--- a/data/plotting_lut.xlsx
+++ b/data/plotting_lut.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="datasets" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="variables" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="variables_mumu" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="variables_ee" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="215">
   <si>
     <t xml:space="preserve">dataset_name</t>
   </si>
@@ -72,6 +73,18 @@
     <t xml:space="preserve">Data (2012D)</t>
   </si>
   <si>
+    <t xml:space="preserve">electron_2012A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">electron_2012B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">electron_2012C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">electron_2012D</t>
+  </si>
+  <si>
     <t xml:space="preserve">ttbar_lep</t>
   </si>
   <si>
@@ -189,7 +202,7 @@
     <t xml:space="preserve">$\sf \bar{t}$ (tW)</t>
   </si>
   <si>
-    <t xml:space="preserve">bprime_Xb</t>
+    <t xml:space="preserve">bprime_xb</t>
   </si>
   <si>
     <t xml:space="preserve">#3451a1</t>
@@ -574,6 +587,87 @@
   </si>
   <si>
     <t xml:space="preserve">|\Delta R(\mu\mu,\, j)|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p_{T}^{e} \, [GeV]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|\Delta\eta(e, e)|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|\Delta\phi(e, e)|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|\Delta R(e, e)|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M_{e,e} \, [GeV]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p_{T}^{e,e} \, [GeV]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\eta_{ee}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\phi_{ee}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p_{T}^{ee}/M_{ee}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M_{ee b} [GeV]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\phi_{ee b}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\eta_{ee b}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p_{T}^{ee b} [GeV]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|\Delta\eta(ee,\, b)|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|\Delta\phi(ee,\, b)|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|\Delta R(ee,\, b)|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M_{e e jj} [GeV]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|\Delta\eta(ee,\, jj)|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|\Delta\phi(ee,\, jj)|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|\Delta R(ee,\, jj)|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M_{eej} [GeV]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\phi_{eej}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\eta_{eej}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p_{T}^{eej} [GeV]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|\Delta\eta(ee,\, j)|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|\Delta\phi(ee,\, j)|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|\Delta R(ee,\, j)|</t>
   </si>
 </sst>
 </file>
@@ -654,13 +748,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -740,21 +838,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H12" activeCellId="1" sqref="2:2 H12"/>
+      <selection pane="bottomLeft" activeCell="H32" activeCellId="0" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.7551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8724489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.9591836734694"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1275510204082"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.0867346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.1836734693878"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.4183673469388"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
   </cols>
@@ -859,409 +957,409 @@
         <v>9</v>
       </c>
     </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>25.81</v>
+        <v>1</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>107.66</v>
+        <v>1</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>3531.9</v>
+        <v>1</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>860.5</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>57.25</v>
+        <v>25.81</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>5.09</v>
+        <v>107.66</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>1.086</v>
+        <v>3531.9</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>2.47</v>
+        <v>860.5</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>0.71</v>
+        <v>57.25</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>3.179</v>
+        <v>5.09</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D16" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="0" t="s">
-        <v>43</v>
-      </c>
       <c r="F16" s="0" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>1.76</v>
+        <v>1.086</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>56.4</v>
+        <v>2.47</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>30.7</v>
+        <v>0.71</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>11.177</v>
+        <v>3.179</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>11.177</v>
+        <v>1.76</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>56.4</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>30.7</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="0" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="C23" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D23" s="0" t="s">
+      <c r="B24" s="0" t="n">
+        <v>11.177</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="E23" s="0" t="s">
+      <c r="F24" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="0" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C25" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" s="1" t="s">
+      <c r="B25" s="0" t="n">
+        <v>11.177</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C26" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D26" s="1" t="s">
+      <c r="F25" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="B27" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C27" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C28" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>31</v>
+      <c r="F27" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="B29" s="1" t="n">
         <v>1</v>
@@ -1270,13 +1368,93 @@
         <v>1</v>
       </c>
       <c r="D29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>44</v>
+      <c r="E31" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1300,51 +1478,51 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D19" activeCellId="1" sqref="2:2 D19"/>
+      <selection pane="bottomLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9387755102041"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3622448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.4540816326531"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5918367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.6938775510204"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.9795918367347"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.1785714285714"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>25</v>
@@ -1356,21 +1534,21 @@
         <v>150</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>30</v>
@@ -1384,21 +1562,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="F4" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="G4" s="0" t="s">
-        <v>77</v>
-      </c>
       <c r="H4" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>30</v>
@@ -1410,21 +1588,21 @@
         <v>4.7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F5" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="0" t="s">
-        <v>77</v>
-      </c>
       <c r="H5" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>50</v>
@@ -1436,21 +1614,21 @@
         <v>0.2</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>25</v>
@@ -1462,21 +1640,21 @@
         <v>150</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>30</v>
@@ -1490,21 +1668,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="F8" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G8" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="G8" s="0" t="s">
-        <v>77</v>
-      </c>
       <c r="H8" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>24</v>
@@ -1516,21 +1694,21 @@
         <v>2.4</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F9" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="G9" s="0" t="s">
-        <v>77</v>
-      </c>
       <c r="H9" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>50</v>
@@ -1542,21 +1720,21 @@
         <v>0.2</v>
       </c>
       <c r="E10" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="H10" s="0" t="s">
         <v>93</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>8</v>
@@ -1568,21 +1746,21 @@
         <v>7.5</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="F11" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G11" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="G11" s="0" t="s">
-        <v>77</v>
-      </c>
       <c r="H11" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>4</v>
@@ -1594,21 +1772,21 @@
         <v>3.5</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="F12" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G12" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="G12" s="0" t="s">
-        <v>77</v>
-      </c>
       <c r="H12" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>4</v>
@@ -1620,21 +1798,21 @@
         <v>3.5</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F13" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G13" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="G13" s="0" t="s">
-        <v>77</v>
-      </c>
       <c r="H13" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>50</v>
@@ -1646,21 +1824,21 @@
         <v>1000</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>30</v>
@@ -1674,21 +1852,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="F15" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="G15" s="0" t="s">
-        <v>77</v>
-      </c>
       <c r="H15" s="0" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>25</v>
@@ -1700,21 +1878,21 @@
         <v>5</v>
       </c>
       <c r="E16" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="H16" s="0" t="s">
         <v>108</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>40</v>
@@ -1726,21 +1904,21 @@
         <v>250</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>25</v>
@@ -1752,21 +1930,21 @@
         <v>5</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="F18" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G18" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="G18" s="0" t="s">
-        <v>77</v>
-      </c>
       <c r="H18" s="0" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>30</v>
@@ -1778,21 +1956,21 @@
         <v>150</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>30</v>
@@ -1806,16 +1984,16 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="F21" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G21" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="G21" s="0" t="s">
-        <v>77</v>
-      </c>
       <c r="H21" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1836,8 +2014,8 @@
   </sheetPr>
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1845,42 +2023,42 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9387755102041"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5918367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.6938775510204"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.9795918367347"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.1785714285714"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>26</v>
@@ -1892,21 +2070,21 @@
         <v>150</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>24</v>
@@ -1918,21 +2096,21 @@
         <v>2.4</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>30</v>
@@ -1946,21 +2124,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>25</v>
@@ -1972,21 +2150,21 @@
         <v>6</v>
       </c>
       <c r="E6" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="G6" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>119</v>
-      </c>
       <c r="H6" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>26</v>
@@ -1998,21 +2176,21 @@
         <v>100</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>24</v>
@@ -2024,21 +2202,21 @@
         <v>2.4</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>30</v>
@@ -2052,21 +2230,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>25</v>
@@ -2078,21 +2256,21 @@
         <v>6</v>
       </c>
       <c r="E10" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="G10" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="F10" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>119</v>
-      </c>
       <c r="H10" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>30</v>
@@ -2104,21 +2282,21 @@
         <v>3</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>30</v>
@@ -2131,21 +2309,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>30</v>
@@ -2157,21 +2335,21 @@
         <v>5</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>29</v>
@@ -2183,21 +2361,21 @@
         <v>70</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>30</v>
@@ -2209,21 +2387,21 @@
         <v>250</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>30</v>
@@ -2235,21 +2413,21 @@
         <v>6</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>30</v>
@@ -2263,21 +2441,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>30</v>
@@ -2289,21 +2467,21 @@
         <v>5</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>45</v>
@@ -2315,21 +2493,21 @@
         <v>500</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>30</v>
@@ -2343,21 +2521,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>24</v>
@@ -2369,21 +2547,21 @@
         <v>2.4</v>
       </c>
       <c r="E22" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G22" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="F22" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>148</v>
-      </c>
       <c r="H22" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>29</v>
@@ -2395,21 +2573,21 @@
         <v>300</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>30</v>
@@ -2421,21 +2599,21 @@
         <v>3</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>30</v>
@@ -2448,21 +2626,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>30</v>
@@ -2474,21 +2652,21 @@
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>45</v>
@@ -2500,21 +2678,21 @@
         <v>1000</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>30</v>
@@ -2526,21 +2704,21 @@
         <v>3</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>30</v>
@@ -2553,21 +2731,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>30</v>
@@ -2579,21 +2757,21 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>25</v>
@@ -2605,21 +2783,21 @@
         <v>550</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>30</v>
@@ -2633,21 +2811,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>24</v>
@@ -2659,21 +2837,21 @@
         <v>2.4</v>
       </c>
       <c r="E35" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="H35" s="0" t="s">
         <v>175</v>
-      </c>
-      <c r="F35" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="G35" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="H35" s="0" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>29</v>
@@ -2685,21 +2863,21 @@
         <v>300</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>30</v>
@@ -2711,21 +2889,21 @@
         <v>3</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>30</v>
@@ -2738,21 +2916,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>30</v>
@@ -2764,16 +2942,974 @@
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G39" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="H39" s="0" t="s">
+        <v>175</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H39"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9387755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.6938775510204"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.1785714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>-2.4</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <f aca="false">-PI()</f>
+        <v>-3.14159265358979</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <f aca="false">PI()</f>
+        <v>3.14159265358979</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>-2.4</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <f aca="false">-PI()</f>
+        <v>-3.14159265358979</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <f aca="false">PI()</f>
+        <v>3.14159265358979</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <f aca="false">PI()</f>
+        <v>3.14159265358979</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>-6</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <f aca="false">-PI()</f>
+        <v>-3.14159265358979</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <f aca="false">PI()</f>
+        <v>3.14159265358979</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
         <v>148</v>
       </c>
+      <c r="B18" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <f aca="false">-PI()</f>
+        <v>-3.14159265358979</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <f aca="false">PI()</f>
+        <v>3.14159265358979</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>-2.4</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <f aca="false">PI()</f>
+        <v>3.14159265358979</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <f aca="false">PI()</f>
+        <v>3.14159265358979</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G31" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="H31" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>550</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="H33" s="0" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <f aca="false">-PI()</f>
+        <v>-3.14159265358979</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <f aca="false">PI()</f>
+        <v>3.14159265358979</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>-2.4</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="H35" s="0" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="H36" s="0" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <f aca="false">PI()</f>
+        <v>3.14159265358979</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="H38" s="0" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>152</v>
+      </c>
       <c r="H39" s="0" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
need to debug normalization for sig_pdf_alt in fit_tools
</commit_message>
<xml_diff>
--- a/data/plotting_lut.xlsx
+++ b/data/plotting_lut.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="datasets" sheetId="1" state="visible" r:id="rId2"/>
@@ -840,7 +840,7 @@
   </sheetPr>
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="H32" activeCellId="0" sqref="H32"/>
@@ -848,11 +848,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8571428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.9591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.9438775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.0612244897959"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1275510204082"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.1836734693878"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.2857142857143"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.4183673469388"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
   </cols>
@@ -1485,12 +1485,12 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9387755102041"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.4540816326531"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.5510204081633"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.6938775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.780612244898"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.1785714285714"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.3673469387755"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -2014,8 +2014,8 @@
   </sheetPr>
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2023,10 +2023,10 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9387755102041"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.6938775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.780612244898"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.1785714285714"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.3673469387755"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -2167,10 +2167,10 @@
         <v>129</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>100</v>
@@ -2981,10 +2981,10 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9387755102041"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.6938775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.780612244898"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.1785714285714"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.3673469387755"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
removed data scaling from amumu_fit
</commit_message>
<xml_diff>
--- a/data/plotting_lut.xlsx
+++ b/data/plotting_lut.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="259">
   <si>
     <t xml:space="preserve">dataset_name</t>
   </si>
@@ -273,6 +273,9 @@
     <t xml:space="preserve">electron_2016D</t>
   </si>
   <si>
+    <t xml:space="preserve">ttjets</t>
+  </si>
+  <si>
     <t xml:space="preserve">variable_name</t>
   </si>
   <si>
@@ -297,6 +300,21 @@
     <t xml:space="preserve">condition</t>
   </si>
   <si>
+    <t xml:space="preserve">n_pu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N_{pu}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entries\,/\, bin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">misc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None</t>
+  </si>
+  <si>
     <t xml:space="preserve">jet_pt</t>
   </si>
   <si>
@@ -361,9 +379,6 @@
   </si>
   <si>
     <t xml:space="preserve">N_{jets}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">None</t>
   </si>
   <si>
     <t xml:space="preserve">n_bjets</t>
@@ -962,16 +977,16 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C27" activeCellId="2" sqref="A2:A9 E2:E9 C27"/>
+      <selection pane="bottomLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.9438775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.2602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1275510204082"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.4744897959184"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.5612244897959"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.4183673469388"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
   </cols>
@@ -1592,19 +1607,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A2:A9 E2:E9"/>
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.9438775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.2602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1275510204082"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.4744897959184"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.5612244897959"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.4183673469388"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
   </cols>
@@ -1791,10 +1806,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>20</v>
+        <v>82</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>25.81</v>
+        <v>831.76</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>1</v>
@@ -1803,7 +1818,7 @@
         <v>21</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>23</v>
@@ -1811,10 +1826,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>107.66</v>
+        <v>25.81</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>1</v>
@@ -1823,7 +1838,7 @@
         <v>21</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>23</v>
@@ -1831,30 +1846,30 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>3531.9</v>
+        <v>107.66</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>860.5</v>
+        <v>5765.4</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>1</v>
@@ -1863,7 +1878,7 @@
         <v>27</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>29</v>
@@ -1871,39 +1886,39 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>57.25</v>
+        <v>18610</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>5.09</v>
+        <v>57.25</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>35</v>
@@ -1911,10 +1926,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>1.086</v>
+        <v>5.595</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>1</v>
@@ -1923,7 +1938,7 @@
         <v>37</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>35</v>
@@ -1931,19 +1946,19 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>2.47</v>
+        <v>5.26</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>35</v>
@@ -1951,10 +1966,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>0.71</v>
+        <v>3.22</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>1</v>
@@ -1963,7 +1978,7 @@
         <v>42</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>35</v>
@@ -1971,10 +1986,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>3.179</v>
+        <v>0.564</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>1</v>
@@ -1983,18 +1998,18 @@
         <v>42</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>1.76</v>
+        <v>10.306</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>1</v>
@@ -2003,7 +2018,7 @@
         <v>42</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>48</v>
@@ -2011,10 +2026,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>56.4</v>
+        <v>1.76</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>1</v>
@@ -2023,7 +2038,7 @@
         <v>42</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>48</v>
@@ -2031,10 +2046,10 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>30.7</v>
+        <v>216.84</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>1</v>
@@ -2043,7 +2058,7 @@
         <v>42</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>48</v>
@@ -2051,10 +2066,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>11.177</v>
+        <v>136</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>1</v>
@@ -2063,7 +2078,7 @@
         <v>42</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>48</v>
@@ -2071,10 +2086,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>11.177</v>
+        <v>35.6</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>1</v>
@@ -2083,55 +2098,55 @@
         <v>42</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>35.6</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="B27" s="0" t="n">
+      <c r="B28" s="0" t="n">
         <v>0.03</v>
       </c>
-      <c r="C27" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D27" s="0" t="s">
+      <c r="C28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="E27" s="0" t="s">
+      <c r="E28" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="F27" s="0" t="s">
+      <c r="F28" s="0" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B29" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C29" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B30" s="1" t="n">
         <v>1</v>
@@ -2140,18 +2155,18 @@
         <v>1</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>63</v>
+        <v>7</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B31" s="1" t="n">
         <v>1</v>
@@ -2160,18 +2175,18 @@
         <v>1</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B32" s="1" t="n">
         <v>1</v>
@@ -2180,32 +2195,52 @@
         <v>1</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C33" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D33" s="1" t="s">
+      <c r="B34" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2225,12 +2260,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D19" activeCellId="2" sqref="A2:A9 E2:E9 D19"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2239,169 +2274,148 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.5510204081633"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.969387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.0714285714286"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.75"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.8520408163265"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>25</v>
+        <v>0.5</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>150</v>
+        <v>80.5</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="C4" s="0" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C6" s="0" t="n">
         <f aca="false">-PI()</f>
         <v>-3.14159265358979</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D6" s="0" t="n">
         <f aca="false">PI()</f>
         <v>3.14159265358979</v>
       </c>
-      <c r="E4" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>-4.7</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="E6" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="G6" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="F5" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="H6" s="0" t="s">
         <v>100</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>-0.2</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>25</v>
+        <v>-4.7</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>150</v>
+        <v>4.7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2409,263 +2423,263 @@
         <v>106</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C8" s="0" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C10" s="0" t="n">
         <f aca="false">-PI()</f>
         <v>-3.14159265358979</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D10" s="0" t="n">
         <f aca="false">PI()</f>
         <v>3.14159265358979</v>
       </c>
-      <c r="E8" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="C9" s="0" t="n">
-        <v>-2.4</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>2.4</v>
-      </c>
-      <c r="E9" s="0" t="s">
+      <c r="E10" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="G10" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="F9" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>-0.2</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>93</v>
-      </c>
       <c r="H10" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>-0.5</v>
+        <v>-2.4</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>7.5</v>
+        <v>2.4</v>
       </c>
       <c r="E11" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="H11" s="0" t="s">
         <v>111</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>-0.5</v>
+        <v>-0.2</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>3.5</v>
+        <v>0.2</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>-0.5</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>3.5</v>
+        <v>7.5</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>1000</v>
+        <v>3.5</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="B15" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="C15" s="0" t="n">
+      <c r="F15" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C17" s="0" t="n">
         <f aca="false">-PI()</f>
         <v>-3.14159265358979</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D17" s="0" t="n">
         <f aca="false">PI()</f>
         <v>3.14159265358979</v>
       </c>
-      <c r="E15" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="B16" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="C16" s="0" t="n">
-        <v>-5</v>
-      </c>
-      <c r="D16" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="E17" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="H17" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="B17" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="C17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" s="0" t="n">
-        <v>250</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2676,7 +2690,7 @@
         <v>25</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>5</v>
@@ -2685,67 +2699,119 @@
         <v>129</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>120</v>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D20" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="E20" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="H20" s="0" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="B21" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="C21" s="0" t="n">
+      <c r="E22" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C23" s="0" t="n">
         <f aca="false">-PI()</f>
         <v>-3.14159265358979</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D23" s="0" t="n">
         <f aca="false">PI()</f>
         <v>3.14159265358979</v>
       </c>
-      <c r="E21" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="G21" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="H21" s="0" t="s">
-        <v>112</v>
+      <c r="E23" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -2766,8 +2832,8 @@
   </sheetPr>
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="2" sqref="A2:A9 E2:E9 F7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2775,42 +2841,42 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9387755102041"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.969387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.0714285714286"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.75"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.8520408163265"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>26</v>
@@ -2822,21 +2888,21 @@
         <v>150</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>24</v>
@@ -2848,21 +2914,21 @@
         <v>2.4</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>30</v>
@@ -2876,21 +2942,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>25</v>
@@ -2902,21 +2968,21 @@
         <v>6</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="F6" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="G6" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="G6" s="0" t="s">
-        <v>135</v>
-      </c>
       <c r="H6" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>35</v>
@@ -2928,21 +2994,21 @@
         <v>80</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>24</v>
@@ -2954,21 +3020,21 @@
         <v>2.4</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>30</v>
@@ -2982,21 +3048,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>25</v>
@@ -3008,21 +3074,21 @@
         <v>6</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="F10" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="G10" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="G10" s="0" t="s">
-        <v>135</v>
-      </c>
       <c r="H10" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>30</v>
@@ -3034,21 +3100,21 @@
         <v>3</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>30</v>
@@ -3061,21 +3127,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>30</v>
@@ -3087,21 +3153,21 @@
         <v>5</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>29</v>
@@ -3113,21 +3179,21 @@
         <v>70</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>30</v>
@@ -3139,21 +3205,21 @@
         <v>250</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>30</v>
@@ -3165,21 +3231,21 @@
         <v>6</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>30</v>
@@ -3193,21 +3259,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>30</v>
@@ -3219,21 +3285,21 @@
         <v>5</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>45</v>
@@ -3245,21 +3311,21 @@
         <v>500</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>30</v>
@@ -3273,21 +3339,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>24</v>
@@ -3299,21 +3365,21 @@
         <v>2.4</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>29</v>
@@ -3325,21 +3391,21 @@
         <v>300</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>30</v>
@@ -3351,21 +3417,21 @@
         <v>3</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>30</v>
@@ -3378,21 +3444,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>30</v>
@@ -3404,21 +3470,21 @@
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>45</v>
@@ -3430,21 +3496,21 @@
         <v>1000</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>30</v>
@@ -3456,21 +3522,21 @@
         <v>3</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>30</v>
@@ -3483,21 +3549,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>30</v>
@@ -3509,21 +3575,21 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>25</v>
@@ -3535,21 +3601,21 @@
         <v>550</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>30</v>
@@ -3563,21 +3629,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>24</v>
@@ -3589,21 +3655,21 @@
         <v>2.4</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>29</v>
@@ -3615,21 +3681,21 @@
         <v>300</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>30</v>
@@ -3641,21 +3707,21 @@
         <v>3</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>30</v>
@@ -3668,21 +3734,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>30</v>
@@ -3694,16 +3760,16 @@
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -3725,7 +3791,7 @@
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E24" activeCellId="2" sqref="A2:A9 E2:E9 E24"/>
+      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3733,42 +3799,42 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9387755102041"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.969387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.0714285714286"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.75"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.8520408163265"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>26</v>
@@ -3780,21 +3846,21 @@
         <v>150</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>24</v>
@@ -3806,21 +3872,21 @@
         <v>2.4</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>30</v>
@@ -3834,21 +3900,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>25</v>
@@ -3860,21 +3926,21 @@
         <v>6</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="F6" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="G6" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="G6" s="0" t="s">
-        <v>135</v>
-      </c>
       <c r="H6" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>26</v>
@@ -3886,21 +3952,21 @@
         <v>100</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>24</v>
@@ -3912,21 +3978,21 @@
         <v>2.4</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>30</v>
@@ -3940,21 +4006,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>25</v>
@@ -3966,21 +4032,21 @@
         <v>6</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="F10" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="G10" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="G10" s="0" t="s">
-        <v>135</v>
-      </c>
       <c r="H10" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>30</v>
@@ -3992,21 +4058,21 @@
         <v>3</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>30</v>
@@ -4019,21 +4085,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>30</v>
@@ -4045,21 +4111,21 @@
         <v>5</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>29</v>
@@ -4071,21 +4137,21 @@
         <v>70</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>30</v>
@@ -4097,21 +4163,21 @@
         <v>250</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>30</v>
@@ -4123,21 +4189,21 @@
         <v>6</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>30</v>
@@ -4151,21 +4217,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>30</v>
@@ -4177,21 +4243,21 @@
         <v>5</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>45</v>
@@ -4203,21 +4269,21 @@
         <v>500</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>30</v>
@@ -4231,21 +4297,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>24</v>
@@ -4257,21 +4323,21 @@
         <v>2.4</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>29</v>
@@ -4283,21 +4349,21 @@
         <v>300</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>30</v>
@@ -4309,21 +4375,21 @@
         <v>3</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>30</v>
@@ -4336,21 +4402,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>30</v>
@@ -4362,21 +4428,21 @@
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>45</v>
@@ -4388,21 +4454,21 @@
         <v>1000</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>30</v>
@@ -4414,21 +4480,21 @@
         <v>3</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>30</v>
@@ -4441,21 +4507,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>30</v>
@@ -4467,21 +4533,21 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>25</v>
@@ -4493,21 +4559,21 @@
         <v>550</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>30</v>
@@ -4521,21 +4587,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>24</v>
@@ -4547,21 +4613,21 @@
         <v>2.4</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>29</v>
@@ -4573,21 +4639,21 @@
         <v>300</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>30</v>
@@ -4599,21 +4665,21 @@
         <v>3</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>30</v>
@@ -4626,21 +4692,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>30</v>
@@ -4652,16 +4718,16 @@
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -4683,7 +4749,7 @@
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E28" activeCellId="2" sqref="A2:A9 E2:E9 E28"/>
+      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4691,42 +4757,42 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9387755102041"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.969387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.0714285714286"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.75"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.8520408163265"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>26</v>
@@ -4738,21 +4804,21 @@
         <v>150</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>24</v>
@@ -4764,21 +4830,21 @@
         <v>2.4</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>30</v>
@@ -4792,21 +4858,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>25</v>
@@ -4818,21 +4884,21 @@
         <v>6</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="F6" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="G6" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="G6" s="0" t="s">
-        <v>135</v>
-      </c>
       <c r="H6" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>36</v>
@@ -4844,21 +4910,21 @@
         <v>100</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>24</v>
@@ -4870,21 +4936,21 @@
         <v>2.4</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>30</v>
@@ -4898,21 +4964,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>25</v>
@@ -4924,21 +4990,21 @@
         <v>6</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="F10" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="G10" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="G10" s="0" t="s">
-        <v>135</v>
-      </c>
       <c r="H10" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>30</v>
@@ -4950,21 +5016,21 @@
         <v>3</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>30</v>
@@ -4977,21 +5043,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>30</v>
@@ -5003,21 +5069,21 @@
         <v>5</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>30</v>
@@ -5029,21 +5095,21 @@
         <v>200</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>30</v>
@@ -5055,21 +5121,21 @@
         <v>250</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>30</v>
@@ -5081,21 +5147,21 @@
         <v>6</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>30</v>
@@ -5109,21 +5175,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>30</v>
@@ -5135,21 +5201,21 @@
         <v>5</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>45</v>
@@ -5161,21 +5227,21 @@
         <v>500</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>30</v>
@@ -5189,21 +5255,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>24</v>
@@ -5215,21 +5281,21 @@
         <v>2.4</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>29</v>
@@ -5241,21 +5307,21 @@
         <v>300</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>30</v>
@@ -5267,21 +5333,21 @@
         <v>3</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>30</v>
@@ -5294,21 +5360,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>30</v>
@@ -5320,21 +5386,21 @@
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>45</v>
@@ -5346,21 +5412,21 @@
         <v>1000</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>30</v>
@@ -5372,21 +5438,21 @@
         <v>3</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>30</v>
@@ -5399,21 +5465,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>30</v>
@@ -5425,21 +5491,21 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>25</v>
@@ -5451,21 +5517,21 @@
         <v>550</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>30</v>
@@ -5479,21 +5545,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>24</v>
@@ -5505,21 +5571,21 @@
         <v>2.4</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>29</v>
@@ -5531,21 +5597,21 @@
         <v>300</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>30</v>
@@ -5557,21 +5623,21 @@
         <v>3</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>30</v>
@@ -5584,21 +5650,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>30</v>
@@ -5610,16 +5676,16 @@
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding in mass resolution notebook
</commit_message>
<xml_diff>
--- a/data/plotting_lut.xlsx
+++ b/data/plotting_lut.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="263">
   <si>
     <t xml:space="preserve">dataset_name</t>
   </si>
@@ -213,6 +213,9 @@
     <t xml:space="preserve">$\sf B’\rightarrow Xb$</t>
   </si>
   <si>
+    <t xml:space="preserve">fcnc</t>
+  </si>
+  <si>
     <t xml:space="preserve">Data</t>
   </si>
   <si>
@@ -237,12 +240,6 @@
     <t xml:space="preserve">#f1ca2d</t>
   </si>
   <si>
-    <t xml:space="preserve">muon_2016A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data (2016A)</t>
-  </si>
-  <si>
     <t xml:space="preserve">muon_2016B</t>
   </si>
   <si>
@@ -261,7 +258,22 @@
     <t xml:space="preserve">Data (2016D)</t>
   </si>
   <si>
-    <t xml:space="preserve">electron_2016A</t>
+    <t xml:space="preserve">muon_2016E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data (2016E)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">muon_2016F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data (2016F)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">muon_2016G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data (2016G)</t>
   </si>
   <si>
     <t xml:space="preserve">electron_2016B</t>
@@ -972,12 +984,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="bottomLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -986,7 +998,7 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1275510204082"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.5612244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.6632653061224"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.4183673469388"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
   </cols>
@@ -1491,29 +1503,30 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B29" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C29" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" s="1" t="s">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>9</v>
+      <c r="B28" s="0" t="n">
+        <f aca="false">252*0.001</f>
+        <v>0.252</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B30" s="1" t="n">
         <v>1</v>
@@ -1522,18 +1535,18 @@
         <v>1</v>
       </c>
       <c r="D30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="F30" s="1" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B31" s="1" t="n">
         <v>1</v>
@@ -1542,18 +1555,18 @@
         <v>1</v>
       </c>
       <c r="D31" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="F31" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B32" s="1" t="n">
         <v>1</v>
@@ -1562,32 +1575,52 @@
         <v>1</v>
       </c>
       <c r="D32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="F32" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C33" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E33" s="1" t="s">
+      <c r="B34" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1607,10 +1640,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1619,7 +1652,7 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1275510204082"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.5612244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.6632653061224"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.4183673469388"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
   </cols>
@@ -1646,7 +1679,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
@@ -1658,7 +1691,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>9</v>
@@ -1666,7 +1699,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -1678,7 +1711,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>9</v>
@@ -1686,7 +1719,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
@@ -1698,7 +1731,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>9</v>
@@ -1706,7 +1739,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1</v>
@@ -1718,7 +1751,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>9</v>
@@ -1726,7 +1759,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1</v>
@@ -1738,7 +1771,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>9</v>
@@ -1746,7 +1779,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1</v>
@@ -1758,7 +1791,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>9</v>
@@ -1766,7 +1799,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>1</v>
@@ -1778,7 +1811,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>9</v>
@@ -1786,7 +1819,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>1</v>
@@ -1798,38 +1831,38 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>831.76</v>
-      </c>
-      <c r="C11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>23</v>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>25.81</v>
+        <v>831.76</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>1</v>
@@ -1838,7 +1871,7 @@
         <v>21</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>23</v>
@@ -1846,10 +1879,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>107.66</v>
+        <v>25.81</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>1</v>
@@ -1858,7 +1891,7 @@
         <v>21</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>23</v>
@@ -1866,30 +1899,30 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>5765.4</v>
+        <v>107.66</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>18610</v>
+        <v>5765.4</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>1</v>
@@ -1898,7 +1931,7 @@
         <v>27</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>29</v>
@@ -1906,39 +1939,39 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>57.25</v>
+        <v>18610</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>5.595</v>
+        <v>57.25</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>35</v>
@@ -1946,10 +1979,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>5.26</v>
+        <v>5.595</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>1</v>
@@ -1958,7 +1991,7 @@
         <v>37</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>35</v>
@@ -1966,19 +1999,19 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>3.22</v>
+        <v>5.26</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>35</v>
@@ -1986,10 +2019,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>0.564</v>
+        <v>3.22</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>1</v>
@@ -1998,7 +2031,7 @@
         <v>42</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>35</v>
@@ -2006,10 +2039,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>10.306</v>
+        <v>0.564</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>1</v>
@@ -2018,18 +2051,18 @@
         <v>42</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>1.76</v>
+        <v>10.306</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>1</v>
@@ -2038,7 +2071,7 @@
         <v>42</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>48</v>
@@ -2046,10 +2079,10 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>216.84</v>
+        <v>1.76</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>1</v>
@@ -2058,7 +2091,7 @@
         <v>42</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>48</v>
@@ -2066,10 +2099,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>136</v>
+        <v>216.84</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>1</v>
@@ -2078,7 +2111,7 @@
         <v>42</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>48</v>
@@ -2086,10 +2119,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>35.6</v>
+        <v>136</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>1</v>
@@ -2098,7 +2131,7 @@
         <v>42</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>48</v>
@@ -2106,7 +2139,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>35.6</v>
@@ -2118,55 +2151,55 @@
         <v>42</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F26" s="0" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>35.6</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="B28" s="0" t="n">
+      <c r="B29" s="0" t="n">
         <v>0.03</v>
       </c>
-      <c r="C28" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D28" s="0" t="s">
+      <c r="C29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="E28" s="0" t="s">
+      <c r="E29" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="F28" s="0" t="s">
+      <c r="F29" s="0" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B30" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C30" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B31" s="1" t="n">
         <v>1</v>
@@ -2175,18 +2208,18 @@
         <v>1</v>
       </c>
       <c r="D31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="F31" s="1" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B32" s="1" t="n">
         <v>1</v>
@@ -2195,18 +2228,18 @@
         <v>1</v>
       </c>
       <c r="D32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="F32" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B33" s="1" t="n">
         <v>1</v>
@@ -2215,32 +2248,52 @@
         <v>1</v>
       </c>
       <c r="D33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="F33" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B34" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C34" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E34" s="1" t="s">
+      <c r="B35" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2274,42 +2327,42 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.5510204081633"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.0714285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.1683673469388"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.8520408163265"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.9387755102041"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>50</v>
@@ -2321,26 +2374,26 @@
         <v>80.5</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>25</v>
@@ -2352,21 +2405,21 @@
         <v>150</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>30</v>
@@ -2380,21 +2433,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="F6" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="G6" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="G6" s="0" t="s">
-        <v>99</v>
-      </c>
       <c r="H6" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>30</v>
@@ -2406,21 +2459,21 @@
         <v>4.7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F7" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="G7" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="G7" s="0" t="s">
-        <v>99</v>
-      </c>
       <c r="H7" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>50</v>
@@ -2432,21 +2485,21 @@
         <v>0.2</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>25</v>
@@ -2458,21 +2511,21 @@
         <v>150</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>30</v>
@@ -2486,21 +2539,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="F10" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="G10" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="G10" s="0" t="s">
-        <v>99</v>
-      </c>
       <c r="H10" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>24</v>
@@ -2512,21 +2565,21 @@
         <v>2.4</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F11" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="G11" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="G11" s="0" t="s">
-        <v>99</v>
-      </c>
       <c r="H11" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>50</v>
@@ -2538,21 +2591,21 @@
         <v>0.2</v>
       </c>
       <c r="E12" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="H12" s="0" t="s">
         <v>115</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>8</v>
@@ -2564,21 +2617,21 @@
         <v>7.5</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="F13" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="G13" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="G13" s="0" t="s">
+      <c r="H13" s="0" t="s">
         <v>99</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>4</v>
@@ -2590,21 +2643,21 @@
         <v>3.5</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="F14" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="G14" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="G14" s="0" t="s">
+      <c r="H14" s="0" t="s">
         <v>99</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>4</v>
@@ -2616,21 +2669,21 @@
         <v>3.5</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="F15" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="G15" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="G15" s="0" t="s">
+      <c r="H15" s="0" t="s">
         <v>99</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>50</v>
@@ -2642,21 +2695,21 @@
         <v>1000</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>30</v>
@@ -2670,21 +2723,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="F17" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="G17" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="G17" s="0" t="s">
-        <v>99</v>
-      </c>
       <c r="H17" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>25</v>
@@ -2696,21 +2749,21 @@
         <v>5</v>
       </c>
       <c r="E18" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="H18" s="0" t="s">
         <v>129</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>40</v>
@@ -2722,21 +2775,21 @@
         <v>250</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>25</v>
@@ -2748,21 +2801,21 @@
         <v>5</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="F20" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="G20" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="G20" s="0" t="s">
-        <v>99</v>
-      </c>
       <c r="H20" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>30</v>
@@ -2774,21 +2827,21 @@
         <v>150</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="G22" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="H22" s="0" t="s">
         <v>99</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>30</v>
@@ -2802,16 +2855,16 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="F23" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="G23" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="G23" s="0" t="s">
+      <c r="H23" s="0" t="s">
         <v>99</v>
-      </c>
-      <c r="H23" s="0" t="s">
-        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -2841,42 +2894,42 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9387755102041"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.0714285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.1683673469388"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.8520408163265"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.9387755102041"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>26</v>
@@ -2888,21 +2941,21 @@
         <v>150</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>24</v>
@@ -2914,21 +2967,21 @@
         <v>2.4</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>30</v>
@@ -2942,21 +2995,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>25</v>
@@ -2968,21 +3021,21 @@
         <v>6</v>
       </c>
       <c r="E6" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="G6" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>140</v>
-      </c>
       <c r="H6" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>35</v>
@@ -2994,21 +3047,21 @@
         <v>80</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>24</v>
@@ -3020,21 +3073,21 @@
         <v>2.4</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>30</v>
@@ -3048,21 +3101,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>25</v>
@@ -3074,21 +3127,21 @@
         <v>6</v>
       </c>
       <c r="E10" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="G10" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="F10" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>140</v>
-      </c>
       <c r="H10" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>30</v>
@@ -3100,21 +3153,21 @@
         <v>3</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>30</v>
@@ -3127,21 +3180,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>30</v>
@@ -3153,21 +3206,21 @@
         <v>5</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>29</v>
@@ -3179,21 +3232,21 @@
         <v>70</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>30</v>
@@ -3205,21 +3258,21 @@
         <v>250</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>30</v>
@@ -3231,21 +3284,21 @@
         <v>6</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>30</v>
@@ -3259,21 +3312,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>30</v>
@@ -3285,21 +3338,21 @@
         <v>5</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>45</v>
@@ -3311,21 +3364,21 @@
         <v>500</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>30</v>
@@ -3339,21 +3392,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>24</v>
@@ -3365,21 +3418,21 @@
         <v>2.4</v>
       </c>
       <c r="E22" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="G22" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="F22" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>169</v>
-      </c>
       <c r="H22" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>29</v>
@@ -3391,21 +3444,21 @@
         <v>300</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>30</v>
@@ -3417,21 +3470,21 @@
         <v>3</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>30</v>
@@ -3444,21 +3497,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>30</v>
@@ -3470,21 +3523,21 @@
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>45</v>
@@ -3496,21 +3549,21 @@
         <v>1000</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>30</v>
@@ -3522,21 +3575,21 @@
         <v>3</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>30</v>
@@ -3549,21 +3602,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>30</v>
@@ -3575,21 +3628,21 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>25</v>
@@ -3601,21 +3654,21 @@
         <v>550</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>30</v>
@@ -3629,21 +3682,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>24</v>
@@ -3655,21 +3708,21 @@
         <v>2.4</v>
       </c>
       <c r="E35" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="H35" s="0" t="s">
         <v>196</v>
-      </c>
-      <c r="F35" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="G35" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="H35" s="0" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>29</v>
@@ -3681,21 +3734,21 @@
         <v>300</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>30</v>
@@ -3707,21 +3760,21 @@
         <v>3</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>30</v>
@@ -3734,21 +3787,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>30</v>
@@ -3760,16 +3813,16 @@
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -3799,42 +3852,42 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9387755102041"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.0714285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.1683673469388"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.8520408163265"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.9387755102041"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>26</v>
@@ -3846,21 +3899,21 @@
         <v>150</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>24</v>
@@ -3872,21 +3925,21 @@
         <v>2.4</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>30</v>
@@ -3900,21 +3953,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>25</v>
@@ -3926,21 +3979,21 @@
         <v>6</v>
       </c>
       <c r="E6" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="G6" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>140</v>
-      </c>
       <c r="H6" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>26</v>
@@ -3952,21 +4005,21 @@
         <v>100</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>24</v>
@@ -3978,21 +4031,21 @@
         <v>2.4</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>30</v>
@@ -4006,21 +4059,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>25</v>
@@ -4032,21 +4085,21 @@
         <v>6</v>
       </c>
       <c r="E10" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="G10" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="F10" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>140</v>
-      </c>
       <c r="H10" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>30</v>
@@ -4058,21 +4111,21 @@
         <v>3</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>30</v>
@@ -4085,21 +4138,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>30</v>
@@ -4111,21 +4164,21 @@
         <v>5</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>29</v>
@@ -4137,21 +4190,21 @@
         <v>70</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>30</v>
@@ -4163,21 +4216,21 @@
         <v>250</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>30</v>
@@ -4189,21 +4242,21 @@
         <v>6</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>30</v>
@@ -4217,21 +4270,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>30</v>
@@ -4243,21 +4296,21 @@
         <v>5</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>45</v>
@@ -4269,21 +4322,21 @@
         <v>500</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>30</v>
@@ -4297,21 +4350,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>24</v>
@@ -4323,21 +4376,21 @@
         <v>2.4</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>29</v>
@@ -4349,21 +4402,21 @@
         <v>300</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>30</v>
@@ -4375,21 +4428,21 @@
         <v>3</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>30</v>
@@ -4402,21 +4455,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>30</v>
@@ -4428,21 +4481,21 @@
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>45</v>
@@ -4454,21 +4507,21 @@
         <v>1000</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>30</v>
@@ -4480,21 +4533,21 @@
         <v>3</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>30</v>
@@ -4507,21 +4560,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>30</v>
@@ -4533,21 +4586,21 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>25</v>
@@ -4559,21 +4612,21 @@
         <v>550</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>30</v>
@@ -4587,21 +4640,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>24</v>
@@ -4613,21 +4666,21 @@
         <v>2.4</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>29</v>
@@ -4639,21 +4692,21 @@
         <v>300</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>30</v>
@@ -4665,21 +4718,21 @@
         <v>3</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>30</v>
@@ -4692,21 +4745,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>30</v>
@@ -4718,16 +4771,16 @@
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -4757,42 +4810,42 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9387755102041"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.0714285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.1683673469388"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.8520408163265"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.9387755102041"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>26</v>
@@ -4804,21 +4857,21 @@
         <v>150</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>24</v>
@@ -4830,21 +4883,21 @@
         <v>2.4</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>30</v>
@@ -4858,21 +4911,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>25</v>
@@ -4884,21 +4937,21 @@
         <v>6</v>
       </c>
       <c r="E6" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="G6" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>140</v>
-      </c>
       <c r="H6" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>36</v>
@@ -4910,21 +4963,21 @@
         <v>100</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>24</v>
@@ -4936,21 +4989,21 @@
         <v>2.4</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>30</v>
@@ -4964,21 +5017,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>25</v>
@@ -4990,21 +5043,21 @@
         <v>6</v>
       </c>
       <c r="E10" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="G10" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="F10" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>140</v>
-      </c>
       <c r="H10" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>30</v>
@@ -5016,21 +5069,21 @@
         <v>3</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>30</v>
@@ -5043,21 +5096,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>30</v>
@@ -5069,21 +5122,21 @@
         <v>5</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>30</v>
@@ -5095,21 +5148,21 @@
         <v>200</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>30</v>
@@ -5121,21 +5174,21 @@
         <v>250</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>30</v>
@@ -5147,21 +5200,21 @@
         <v>6</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>30</v>
@@ -5175,21 +5228,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>30</v>
@@ -5201,21 +5254,21 @@
         <v>5</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>45</v>
@@ -5227,21 +5280,21 @@
         <v>500</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>30</v>
@@ -5255,21 +5308,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>24</v>
@@ -5281,21 +5334,21 @@
         <v>2.4</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>29</v>
@@ -5307,21 +5360,21 @@
         <v>300</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>30</v>
@@ -5333,21 +5386,21 @@
         <v>3</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>30</v>
@@ -5360,21 +5413,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>30</v>
@@ -5386,21 +5439,21 @@
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>45</v>
@@ -5412,21 +5465,21 @@
         <v>1000</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>30</v>
@@ -5438,21 +5491,21 @@
         <v>3</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>30</v>
@@ -5465,21 +5518,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>30</v>
@@ -5491,21 +5544,21 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>25</v>
@@ -5517,21 +5570,21 @@
         <v>550</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>30</v>
@@ -5545,21 +5598,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>24</v>
@@ -5571,21 +5624,21 @@
         <v>2.4</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>29</v>
@@ -5597,21 +5650,21 @@
         <v>300</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>30</v>
@@ -5623,21 +5676,21 @@
         <v>3</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>30</v>
@@ -5650,21 +5703,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>30</v>
@@ -5676,16 +5729,16 @@
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding GV notebook; miscellaneous updates
</commit_message>
<xml_diff>
--- a/data/plotting_lut.xlsx
+++ b/data/plotting_lut.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="datasets_2012" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="265">
   <si>
     <t xml:space="preserve">dataset_name</t>
   </si>
@@ -214,6 +214,12 @@
   </si>
   <si>
     <t xml:space="preserve">fcnc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#ed418d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$\sf t\rightarrow hc$</t>
   </si>
   <si>
     <t xml:space="preserve">Data</t>
@@ -986,10 +992,10 @@
   </sheetPr>
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
+      <selection pane="bottomLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1508,17 +1514,16 @@
         <v>62</v>
       </c>
       <c r="B28" s="0" t="n">
-        <f aca="false">252*0.001</f>
-        <v>0.252</v>
+        <v>0.5</v>
       </c>
       <c r="C28" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F28" s="0" t="s">
         <v>62</v>
@@ -1538,7 +1543,7 @@
         <v>7</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>9</v>
@@ -1555,10 +1560,10 @@
         <v>1</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>23</v>
@@ -1575,10 +1580,10 @@
         <v>1</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>29</v>
@@ -1595,10 +1600,10 @@
         <v>1</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>35</v>
@@ -1615,7 +1620,7 @@
         <v>1</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>48</v>
@@ -1642,8 +1647,8 @@
   </sheetPr>
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1679,7 +1684,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
@@ -1691,7 +1696,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>9</v>
@@ -1699,7 +1704,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -1711,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>9</v>
@@ -1719,7 +1724,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
@@ -1731,7 +1736,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>9</v>
@@ -1739,7 +1744,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1</v>
@@ -1751,7 +1756,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>9</v>
@@ -1759,7 +1764,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1</v>
@@ -1771,7 +1776,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>9</v>
@@ -1779,7 +1784,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1</v>
@@ -1791,7 +1796,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>9</v>
@@ -1799,7 +1804,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>1</v>
@@ -1811,7 +1816,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>9</v>
@@ -1819,7 +1824,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>1</v>
@@ -1831,7 +1836,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>9</v>
@@ -1839,7 +1844,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>1</v>
@@ -1851,7 +1856,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>9</v>
@@ -1859,7 +1864,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>831.76</v>
@@ -1871,7 +1876,7 @@
         <v>21</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>23</v>
@@ -2211,7 +2216,7 @@
         <v>7</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>9</v>
@@ -2228,10 +2233,10 @@
         <v>1</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>23</v>
@@ -2248,10 +2253,10 @@
         <v>1</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>29</v>
@@ -2268,10 +2273,10 @@
         <v>1</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>35</v>
@@ -2288,7 +2293,7 @@
         <v>1</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>48</v>
@@ -2336,33 +2341,33 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>50</v>
@@ -2374,26 +2379,26 @@
         <v>80.5</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>25</v>
@@ -2405,21 +2410,21 @@
         <v>150</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>30</v>
@@ -2433,21 +2438,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E6" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="H6" s="0" t="s">
         <v>106</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>30</v>
@@ -2459,21 +2464,21 @@
         <v>4.7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>50</v>
@@ -2485,21 +2490,21 @@
         <v>0.2</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>25</v>
@@ -2511,21 +2516,21 @@
         <v>150</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>30</v>
@@ -2539,21 +2544,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>24</v>
@@ -2565,21 +2570,21 @@
         <v>2.4</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>50</v>
@@ -2591,21 +2596,21 @@
         <v>0.2</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>8</v>
@@ -2617,21 +2622,21 @@
         <v>7.5</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>4</v>
@@ -2643,21 +2648,21 @@
         <v>3.5</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>4</v>
@@ -2669,21 +2674,21 @@
         <v>3.5</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>50</v>
@@ -2695,21 +2700,21 @@
         <v>1000</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>30</v>
@@ -2723,21 +2728,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E17" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="H17" s="0" t="s">
         <v>131</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>25</v>
@@ -2749,21 +2754,21 @@
         <v>5</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>40</v>
@@ -2775,21 +2780,21 @@
         <v>250</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>25</v>
@@ -2801,21 +2806,21 @@
         <v>5</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>30</v>
@@ -2827,21 +2832,21 @@
         <v>150</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>30</v>
@@ -2855,16 +2860,16 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2903,33 +2908,33 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>26</v>
@@ -2941,21 +2946,21 @@
         <v>150</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>24</v>
@@ -2967,21 +2972,21 @@
         <v>2.4</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>30</v>
@@ -2995,21 +3000,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>25</v>
@@ -3021,21 +3026,21 @@
         <v>6</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>35</v>
@@ -3047,21 +3052,21 @@
         <v>80</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>24</v>
@@ -3073,21 +3078,21 @@
         <v>2.4</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>30</v>
@@ -3101,21 +3106,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>25</v>
@@ -3127,21 +3132,21 @@
         <v>6</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>30</v>
@@ -3153,21 +3158,21 @@
         <v>3</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>30</v>
@@ -3180,21 +3185,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>30</v>
@@ -3206,21 +3211,21 @@
         <v>5</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>29</v>
@@ -3232,21 +3237,21 @@
         <v>70</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>30</v>
@@ -3258,21 +3263,21 @@
         <v>250</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>30</v>
@@ -3284,21 +3289,21 @@
         <v>6</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>30</v>
@@ -3312,21 +3317,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>30</v>
@@ -3338,21 +3343,21 @@
         <v>5</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>45</v>
@@ -3364,21 +3369,21 @@
         <v>500</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>30</v>
@@ -3392,21 +3397,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E21" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="G21" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="F21" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="G21" s="0" t="s">
-        <v>173</v>
-      </c>
       <c r="H21" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>24</v>
@@ -3418,21 +3423,21 @@
         <v>2.4</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>29</v>
@@ -3444,21 +3449,21 @@
         <v>300</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>30</v>
@@ -3470,21 +3475,21 @@
         <v>3</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>30</v>
@@ -3497,21 +3502,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>30</v>
@@ -3523,21 +3528,21 @@
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>45</v>
@@ -3549,21 +3554,21 @@
         <v>1000</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>30</v>
@@ -3575,21 +3580,21 @@
         <v>3</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>30</v>
@@ -3602,21 +3607,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>30</v>
@@ -3628,21 +3633,21 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>25</v>
@@ -3654,21 +3659,21 @@
         <v>550</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>30</v>
@@ -3682,21 +3687,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E34" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="H34" s="0" t="s">
         <v>198</v>
-      </c>
-      <c r="F34" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="G34" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="H34" s="0" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>24</v>
@@ -3708,21 +3713,21 @@
         <v>2.4</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>29</v>
@@ -3734,21 +3739,21 @@
         <v>300</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>30</v>
@@ -3760,21 +3765,21 @@
         <v>3</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>30</v>
@@ -3787,21 +3792,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>30</v>
@@ -3813,16 +3818,16 @@
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -3861,33 +3866,33 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>26</v>
@@ -3899,21 +3904,21 @@
         <v>150</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>24</v>
@@ -3925,21 +3930,21 @@
         <v>2.4</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>30</v>
@@ -3953,21 +3958,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>25</v>
@@ -3979,21 +3984,21 @@
         <v>6</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>26</v>
@@ -4005,21 +4010,21 @@
         <v>100</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>24</v>
@@ -4031,21 +4036,21 @@
         <v>2.4</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>30</v>
@@ -4059,21 +4064,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>25</v>
@@ -4085,21 +4090,21 @@
         <v>6</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>30</v>
@@ -4111,21 +4116,21 @@
         <v>3</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>30</v>
@@ -4138,21 +4143,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>30</v>
@@ -4164,21 +4169,21 @@
         <v>5</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>29</v>
@@ -4190,21 +4195,21 @@
         <v>70</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>30</v>
@@ -4216,21 +4221,21 @@
         <v>250</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>30</v>
@@ -4242,21 +4247,21 @@
         <v>6</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>30</v>
@@ -4270,21 +4275,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>30</v>
@@ -4296,21 +4301,21 @@
         <v>5</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>45</v>
@@ -4322,21 +4327,21 @@
         <v>500</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>30</v>
@@ -4350,21 +4355,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>24</v>
@@ -4376,21 +4381,21 @@
         <v>2.4</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>29</v>
@@ -4402,21 +4407,21 @@
         <v>300</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>30</v>
@@ -4428,21 +4433,21 @@
         <v>3</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>30</v>
@@ -4455,21 +4460,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>30</v>
@@ -4481,21 +4486,21 @@
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>45</v>
@@ -4507,21 +4512,21 @@
         <v>1000</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>30</v>
@@ -4533,21 +4538,21 @@
         <v>3</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>30</v>
@@ -4560,21 +4565,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>30</v>
@@ -4586,21 +4591,21 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>25</v>
@@ -4612,21 +4617,21 @@
         <v>550</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>30</v>
@@ -4640,21 +4645,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>24</v>
@@ -4666,21 +4671,21 @@
         <v>2.4</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>29</v>
@@ -4692,21 +4697,21 @@
         <v>300</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>30</v>
@@ -4718,21 +4723,21 @@
         <v>3</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>30</v>
@@ -4745,21 +4750,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>30</v>
@@ -4771,16 +4776,16 @@
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -4819,33 +4824,33 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>26</v>
@@ -4857,21 +4862,21 @@
         <v>150</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>24</v>
@@ -4883,21 +4888,21 @@
         <v>2.4</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>30</v>
@@ -4911,21 +4916,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>25</v>
@@ -4937,21 +4942,21 @@
         <v>6</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>36</v>
@@ -4963,21 +4968,21 @@
         <v>100</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>24</v>
@@ -4989,21 +4994,21 @@
         <v>2.4</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>30</v>
@@ -5017,21 +5022,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>25</v>
@@ -5043,21 +5048,21 @@
         <v>6</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>30</v>
@@ -5069,21 +5074,21 @@
         <v>3</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>30</v>
@@ -5096,21 +5101,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>30</v>
@@ -5122,21 +5127,21 @@
         <v>5</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>30</v>
@@ -5148,21 +5153,21 @@
         <v>200</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>30</v>
@@ -5174,21 +5179,21 @@
         <v>250</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>30</v>
@@ -5200,21 +5205,21 @@
         <v>6</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>30</v>
@@ -5228,21 +5233,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>30</v>
@@ -5254,21 +5259,21 @@
         <v>5</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>45</v>
@@ -5280,21 +5285,21 @@
         <v>500</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>30</v>
@@ -5308,21 +5313,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>24</v>
@@ -5334,21 +5339,21 @@
         <v>2.4</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>29</v>
@@ -5360,21 +5365,21 @@
         <v>300</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>30</v>
@@ -5386,21 +5391,21 @@
         <v>3</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>30</v>
@@ -5413,21 +5418,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>30</v>
@@ -5439,21 +5444,21 @@
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>45</v>
@@ -5465,21 +5470,21 @@
         <v>1000</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>30</v>
@@ -5491,21 +5496,21 @@
         <v>3</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>30</v>
@@ -5518,21 +5523,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>30</v>
@@ -5544,21 +5549,21 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>25</v>
@@ -5570,21 +5575,21 @@
         <v>550</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>30</v>
@@ -5598,21 +5603,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>24</v>
@@ -5624,21 +5629,21 @@
         <v>2.4</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>29</v>
@@ -5650,21 +5655,21 @@
         <v>300</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>30</v>
@@ -5676,21 +5681,21 @@
         <v>3</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>30</v>
@@ -5703,21 +5708,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>30</v>
@@ -5729,16 +5734,16 @@
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding a bunch of notebooks
</commit_message>
<xml_diff>
--- a/data/plotting_lut.xlsx
+++ b/data/plotting_lut.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="datasets_2012" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="293">
   <si>
     <t xml:space="preserve">dataset_name</t>
   </si>
@@ -261,6 +261,15 @@
     <t xml:space="preserve">$\sf B’\rightarrow Xb$</t>
   </si>
   <si>
+    <t xml:space="preserve">bprime_xbxb_semilep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#b9516c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$\sf B’B’\rightarrow XbXb$</t>
+  </si>
+  <si>
     <t xml:space="preserve">fcnc</t>
   </si>
   <si>
@@ -459,6 +468,27 @@
     <t xml:space="preserve">N_{forward jets}</t>
   </si>
   <si>
+    <t xml:space="preserve">jet_delta_eta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|\Delta\eta(b, j)|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_bjets &gt; 0 and (n_jets &gt; 0 or n_fwdjets &gt; 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jet_delta_phi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|\Delta\phi(b, j)|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jet_delta_r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\Delta R(b, j)</t>
+  </si>
+  <si>
     <t xml:space="preserve">dijet_mass</t>
   </si>
   <si>
@@ -466,9 +496,6 @@
   </si>
   <si>
     <t xml:space="preserve">Entries \,/\, 25 \, GeV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n_bjets &gt; 0 and (n_jets &gt; 0 or n_fwdjets &gt; 0)</t>
   </si>
   <si>
     <t xml:space="preserve">dijet_phi</t>
@@ -1047,12 +1074,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
+      <selection pane="bottomLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1061,7 +1088,7 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1275510204082"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.0510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.1377551020408"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.4183673469388"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
   </cols>
@@ -1711,7 +1738,7 @@
         <v>75</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>0.03</v>
+        <v>0.053</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>1</v>
@@ -1731,7 +1758,7 @@
         <v>78</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="C36" s="0" t="n">
         <v>1</v>
@@ -1746,29 +1773,29 @@
         <v>78</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B38" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C38" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E38" s="1" t="s">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>9</v>
+      <c r="B37" s="0" t="n">
+        <v>0.084</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B39" s="1" t="n">
         <v>1</v>
@@ -1777,18 +1804,18 @@
         <v>1</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>82</v>
+        <v>7</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B40" s="1" t="n">
         <v>1</v>
@@ -1797,18 +1824,18 @@
         <v>1</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="B41" s="1" t="n">
         <v>1</v>
@@ -1817,32 +1844,52 @@
         <v>1</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C42" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B42" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C42" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E42" s="1" t="s">
+      <c r="B43" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C43" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1865,7 +1912,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1874,7 +1921,7 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1275510204082"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.0510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.1377551020408"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.4183673469388"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
   </cols>
@@ -1901,7 +1948,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
@@ -1913,7 +1960,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>9</v>
@@ -1921,7 +1968,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -1933,7 +1980,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>9</v>
@@ -1941,7 +1988,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
@@ -1953,7 +2000,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>9</v>
@@ -1961,7 +2008,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1</v>
@@ -1973,7 +2020,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>9</v>
@@ -1981,7 +2028,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1</v>
@@ -1993,7 +2040,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>9</v>
@@ -2001,7 +2048,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1</v>
@@ -2013,7 +2060,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>9</v>
@@ -2021,7 +2068,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>1</v>
@@ -2033,7 +2080,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>9</v>
@@ -2041,7 +2088,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>1</v>
@@ -2053,7 +2100,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>9</v>
@@ -2061,7 +2108,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>1</v>
@@ -2073,7 +2120,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>9</v>
@@ -2081,7 +2128,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>831.76</v>
@@ -2093,7 +2140,7 @@
         <v>21</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>23</v>
@@ -2144,7 +2191,8 @@
         <v>26</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>5765.4</v>
+        <f aca="false">1.05*5765.4</f>
+        <v>6053.67</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>1</v>
@@ -2164,7 +2212,8 @@
         <v>38</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>18610</v>
+        <f aca="false">1.05*18610</f>
+        <v>19540.5</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>1</v>
@@ -2433,7 +2482,7 @@
         <v>7</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>9</v>
@@ -2450,10 +2499,10 @@
         <v>1</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>23</v>
@@ -2470,10 +2519,10 @@
         <v>1</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>29</v>
@@ -2490,10 +2539,10 @@
         <v>1</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>51</v>
@@ -2510,7 +2559,7 @@
         <v>1</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>64</v>
@@ -2535,12 +2584,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2549,42 +2598,42 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.5510204081633"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.5459183673469"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.515306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.7040816326531"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>50</v>
@@ -2596,26 +2645,21 @@
         <v>80.5</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>25</v>
@@ -2627,21 +2671,21 @@
         <v>150</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>30</v>
@@ -2655,21 +2699,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E6" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="G6" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="H6" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>30</v>
@@ -2681,21 +2725,21 @@
         <v>4.7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="F7" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="H7" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>50</v>
@@ -2707,21 +2751,21 @@
         <v>0.2</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>25</v>
@@ -2733,21 +2777,21 @@
         <v>150</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>30</v>
@@ -2761,21 +2805,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E10" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="G10" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="F10" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>121</v>
-      </c>
       <c r="H10" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>24</v>
@@ -2787,21 +2831,21 @@
         <v>2.4</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>50</v>
@@ -2813,21 +2857,21 @@
         <v>0.2</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>8</v>
@@ -2839,21 +2883,21 @@
         <v>7.5</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>4</v>
@@ -2865,21 +2909,21 @@
         <v>3.5</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>4</v>
@@ -2891,101 +2935,100 @@
         <v>3.5</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>1000</v>
+        <v>3</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>30</v>
       </c>
       <c r="C17" s="0" t="n">
-        <f aca="false">-PI()</f>
-        <v>-3.14159265358979</v>
+        <v>0</v>
       </c>
       <c r="D17" s="0" t="n">
         <f aca="false">PI()</f>
         <v>3.14159265358979</v>
       </c>
       <c r="E17" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="H17" s="0" t="s">
         <v>149</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>5</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>40</v>
@@ -2994,125 +3037,205 @@
         <v>0</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>250</v>
+        <v>1000</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B20" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <f aca="false">-PI()</f>
+        <v>-3.14159265358979</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <f aca="false">PI()</f>
+        <v>3.14159265358979</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B21" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="C20" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" s="0" t="n">
+      <c r="C21" s="0" t="n">
+        <v>-5</v>
+      </c>
+      <c r="D21" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="E20" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="H20" s="0" t="s">
-        <v>147</v>
+      <c r="E21" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>120</v>
+        <v>163</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>117</v>
+        <v>149</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C26" s="0" t="n">
         <f aca="false">-PI()</f>
         <v>-3.14159265358979</v>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="D26" s="0" t="n">
         <f aca="false">PI()</f>
         <v>3.14159265358979</v>
       </c>
-      <c r="E23" s="0" t="s">
+      <c r="E26" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="G26" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="F23" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="G23" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="H23" s="0" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="B25" s="0" t="n">
+      <c r="H26" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="B28" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C25" s="0" t="n">
+      <c r="C28" s="0" t="n">
         <v>-0.5</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="D28" s="0" t="n">
         <v>4.5</v>
       </c>
-      <c r="E25" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="F25" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="G25" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="H25" s="0" t="s">
-        <v>117</v>
+      <c r="E28" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -3134,7 +3257,7 @@
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F30" activeCellId="0" sqref="F30"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3142,42 +3265,42 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9387755102041"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.5459183673469"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.515306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.7040816326531"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>26</v>
@@ -3189,21 +3312,21 @@
         <v>150</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="F3" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>120</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>24</v>
@@ -3215,21 +3338,21 @@
         <v>2.4</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>30</v>
@@ -3243,21 +3366,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>25</v>
@@ -3269,21 +3392,21 @@
         <v>6</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>35</v>
@@ -3295,21 +3418,21 @@
         <v>90</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>24</v>
@@ -3321,21 +3444,21 @@
         <v>2.4</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>30</v>
@@ -3349,21 +3472,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>25</v>
@@ -3375,21 +3498,21 @@
         <v>6</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>30</v>
@@ -3401,21 +3524,21 @@
         <v>3</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>30</v>
@@ -3428,21 +3551,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>30</v>
@@ -3454,21 +3577,21 @@
         <v>5</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>29</v>
@@ -3480,21 +3603,21 @@
         <v>70</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>30</v>
@@ -3506,21 +3629,21 @@
         <v>250</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>30</v>
@@ -3532,21 +3655,21 @@
         <v>6</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>30</v>
@@ -3560,21 +3683,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>30</v>
@@ -3586,21 +3709,21 @@
         <v>5</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>45</v>
@@ -3612,21 +3735,21 @@
         <v>500</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>30</v>
@@ -3640,21 +3763,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>24</v>
@@ -3666,21 +3789,21 @@
         <v>2.4</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>29</v>
@@ -3692,21 +3815,21 @@
         <v>300</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>30</v>
@@ -3718,21 +3841,21 @@
         <v>3</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>30</v>
@@ -3745,21 +3868,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>30</v>
@@ -3771,21 +3894,21 @@
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>36</v>
@@ -3797,21 +3920,21 @@
         <v>1000</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>30</v>
@@ -3823,21 +3946,21 @@
         <v>3</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>30</v>
@@ -3850,21 +3973,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>30</v>
@@ -3876,21 +3999,21 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>25</v>
@@ -3902,21 +4025,21 @@
         <v>550</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>30</v>
@@ -3930,21 +4053,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>24</v>
@@ -3956,21 +4079,21 @@
         <v>2.4</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>221</v>
+        <v>230</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>29</v>
@@ -3982,21 +4105,21 @@
         <v>300</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>30</v>
@@ -4008,21 +4131,21 @@
         <v>3</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>30</v>
@@ -4035,21 +4158,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>30</v>
@@ -4061,16 +4184,16 @@
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -4100,42 +4223,42 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9387755102041"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.5459183673469"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.515306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.7040816326531"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>26</v>
@@ -4147,21 +4270,21 @@
         <v>150</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="F3" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>120</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>24</v>
@@ -4173,21 +4296,21 @@
         <v>2.4</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>30</v>
@@ -4201,21 +4324,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>25</v>
@@ -4227,21 +4350,21 @@
         <v>6</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>26</v>
@@ -4253,21 +4376,21 @@
         <v>100</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="F7" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="H7" s="0" t="s">
         <v>120</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>24</v>
@@ -4279,21 +4402,21 @@
         <v>2.4</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>30</v>
@@ -4307,21 +4430,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>25</v>
@@ -4333,21 +4456,21 @@
         <v>6</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>30</v>
@@ -4359,21 +4482,21 @@
         <v>3</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>30</v>
@@ -4386,21 +4509,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>30</v>
@@ -4412,21 +4535,21 @@
         <v>5</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>29</v>
@@ -4438,21 +4561,21 @@
         <v>70</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>30</v>
@@ -4464,21 +4587,21 @@
         <v>250</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>30</v>
@@ -4490,21 +4613,21 @@
         <v>6</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>30</v>
@@ -4518,21 +4641,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>30</v>
@@ -4544,21 +4667,21 @@
         <v>5</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>45</v>
@@ -4570,21 +4693,21 @@
         <v>500</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>238</v>
+        <v>247</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>30</v>
@@ -4598,21 +4721,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>239</v>
+        <v>248</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>24</v>
@@ -4624,21 +4747,21 @@
         <v>2.4</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>29</v>
@@ -4650,21 +4773,21 @@
         <v>300</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>30</v>
@@ -4676,21 +4799,21 @@
         <v>3</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>30</v>
@@ -4703,21 +4826,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>243</v>
+        <v>252</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>30</v>
@@ -4729,21 +4852,21 @@
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>45</v>
@@ -4755,21 +4878,21 @@
         <v>1000</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>30</v>
@@ -4781,21 +4904,21 @@
         <v>3</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>30</v>
@@ -4808,21 +4931,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>30</v>
@@ -4834,21 +4957,21 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>249</v>
+        <v>258</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>25</v>
@@ -4860,21 +4983,21 @@
         <v>550</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>30</v>
@@ -4888,21 +5011,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>24</v>
@@ -4914,21 +5037,21 @@
         <v>2.4</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>221</v>
+        <v>230</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>29</v>
@@ -4940,21 +5063,21 @@
         <v>300</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>253</v>
+        <v>262</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>30</v>
@@ -4966,21 +5089,21 @@
         <v>3</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>30</v>
@@ -4993,21 +5116,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>30</v>
@@ -5019,16 +5142,16 @@
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -5058,42 +5181,42 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9387755102041"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.5459183673469"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.515306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.7040816326531"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>26</v>
@@ -5105,21 +5228,21 @@
         <v>150</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="F3" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>120</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>24</v>
@@ -5131,21 +5254,21 @@
         <v>2.4</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>30</v>
@@ -5159,21 +5282,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>25</v>
@@ -5185,21 +5308,21 @@
         <v>6</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>36</v>
@@ -5211,21 +5334,21 @@
         <v>100</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>24</v>
@@ -5237,21 +5360,21 @@
         <v>2.4</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>30</v>
@@ -5265,21 +5388,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>25</v>
@@ -5291,21 +5414,21 @@
         <v>6</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>30</v>
@@ -5317,21 +5440,21 @@
         <v>3</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>30</v>
@@ -5344,21 +5467,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>30</v>
@@ -5370,21 +5493,21 @@
         <v>5</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>30</v>
@@ -5396,21 +5519,21 @@
         <v>200</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
       <c r="F14" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="H14" s="0" t="s">
         <v>120</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>30</v>
@@ -5422,21 +5545,21 @@
         <v>250</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>262</v>
+        <v>271</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>30</v>
@@ -5448,21 +5571,21 @@
         <v>6</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>30</v>
@@ -5476,21 +5599,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>30</v>
@@ -5502,21 +5625,21 @@
         <v>5</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>45</v>
@@ -5528,21 +5651,21 @@
         <v>500</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>30</v>
@@ -5556,21 +5679,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>24</v>
@@ -5582,21 +5705,21 @@
         <v>2.4</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>29</v>
@@ -5608,21 +5731,21 @@
         <v>300</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>30</v>
@@ -5634,21 +5757,21 @@
         <v>3</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>30</v>
@@ -5661,21 +5784,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>30</v>
@@ -5687,21 +5810,21 @@
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>45</v>
@@ -5713,21 +5836,21 @@
         <v>1000</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>30</v>
@@ -5739,21 +5862,21 @@
         <v>3</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>30</v>
@@ -5766,21 +5889,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>30</v>
@@ -5792,21 +5915,21 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>25</v>
@@ -5818,21 +5941,21 @@
         <v>550</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>30</v>
@@ -5846,21 +5969,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>278</v>
+        <v>287</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>24</v>
@@ -5872,21 +5995,21 @@
         <v>2.4</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>279</v>
+        <v>288</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>221</v>
+        <v>230</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>29</v>
@@ -5898,21 +6021,21 @@
         <v>300</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>280</v>
+        <v>289</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>30</v>
@@ -5924,21 +6047,21 @@
         <v>3</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>281</v>
+        <v>290</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>30</v>
@@ -5951,21 +6074,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>282</v>
+        <v>291</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>30</v>
@@ -5977,16 +6100,16 @@
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>283</v>
+        <v>292</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added weighting sampling in mc mixer
</commit_message>
<xml_diff>
--- a/data/plotting_lut.xlsx
+++ b/data/plotting_lut.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="datasets_2012" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="298">
   <si>
     <t xml:space="preserve">dataset_name</t>
   </si>
@@ -586,6 +586,12 @@
   </si>
   <si>
     <t xml:space="preserve">lepton2_iso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lepton2_cos_theta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\cos (\theta)</t>
   </si>
   <si>
     <t xml:space="preserve">lepton_delta_eta</t>
@@ -1086,9 +1092,9 @@
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="B24" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="B17" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
+      <selection pane="bottomLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1097,7 +1103,7 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1275510204082"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.1377551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.3265306122449"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.4183673469388"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
   </cols>
@@ -1747,7 +1753,7 @@
         <v>75</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>0.045</v>
+        <v>0.05</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>1</v>
@@ -1951,7 +1957,7 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1275510204082"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.1377551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.3265306122449"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.4183673469388"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
   </cols>
@@ -2631,7 +2637,7 @@
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.5459183673469"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.7040816326531"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.0918367346939"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -3284,10 +3290,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3298,7 +3304,7 @@
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.5459183673469"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.7040816326531"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.0918367346939"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -3545,13 +3551,13 @@
         <v>187</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>188</v>
@@ -3563,7 +3569,7 @@
         <v>176</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3577,8 +3583,7 @@
         <v>0</v>
       </c>
       <c r="D12" s="0" t="n">
-        <f aca="false">PI()</f>
-        <v>3.14159265358979</v>
+        <v>3</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>190</v>
@@ -3604,7 +3609,8 @@
         <v>0</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>5</v>
+        <f aca="false">PI()</f>
+        <v>3.14159265358979</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>192</v>
@@ -3624,19 +3630,19 @@
         <v>193</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>194</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>183</v>
+        <v>131</v>
       </c>
       <c r="G14" s="0" t="s">
         <v>176</v>
@@ -3650,19 +3656,19 @@
         <v>195</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>250</v>
+        <v>70</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>196</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>166</v>
+        <v>183</v>
       </c>
       <c r="G15" s="0" t="s">
         <v>176</v>
@@ -3679,16 +3685,16 @@
         <v>30</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>-6</v>
+        <v>0</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>6</v>
+        <v>250</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>198</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>131</v>
+        <v>166</v>
       </c>
       <c r="G16" s="0" t="s">
         <v>176</v>
@@ -3705,12 +3711,10 @@
         <v>30</v>
       </c>
       <c r="C17" s="0" t="n">
-        <f aca="false">-PI()</f>
-        <v>-3.14159265358979</v>
+        <v>-6</v>
       </c>
       <c r="D17" s="0" t="n">
-        <f aca="false">PI()</f>
-        <v>3.14159265358979</v>
+        <v>6</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>200</v>
@@ -3733,10 +3737,12 @@
         <v>30</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>0</v>
+        <f aca="false">-PI()</f>
+        <v>-3.14159265358979</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>5</v>
+        <f aca="false">PI()</f>
+        <v>3.14159265358979</v>
       </c>
       <c r="E18" s="0" t="s">
         <v>202</v>
@@ -3751,55 +3757,53 @@
         <v>123</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
         <v>203</v>
       </c>
-      <c r="B20" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="C20" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="D20" s="0" t="n">
-        <v>500</v>
-      </c>
-      <c r="E20" s="0" t="s">
+      <c r="B19" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E19" s="0" t="s">
         <v>204</v>
       </c>
-      <c r="F20" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="H20" s="0" t="s">
-        <v>139</v>
+      <c r="F19" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="E21" s="0" t="s">
         <v>206</v>
       </c>
-      <c r="B21" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="C21" s="0" t="n">
-        <f aca="false">-PI()</f>
-        <v>-3.14159265358979</v>
-      </c>
-      <c r="D21" s="0" t="n">
-        <f aca="false">PI()</f>
-        <v>3.14159265358979</v>
-      </c>
-      <c r="E21" s="0" t="s">
+      <c r="F21" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="G21" s="0" t="s">
         <v>207</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="G21" s="0" t="s">
-        <v>205</v>
       </c>
       <c r="H21" s="0" t="s">
         <v>139</v>
@@ -3810,13 +3814,15 @@
         <v>208</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>-2.4</v>
+        <f aca="false">-PI()</f>
+        <v>-3.14159265358979</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>2.4</v>
+        <f aca="false">PI()</f>
+        <v>3.14159265358979</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>209</v>
@@ -3825,7 +3831,7 @@
         <v>131</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H22" s="0" t="s">
         <v>139</v>
@@ -3836,22 +3842,22 @@
         <v>210</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>10</v>
+        <v>-2.4</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>300</v>
+        <v>2.4</v>
       </c>
       <c r="E23" s="0" t="s">
         <v>211</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H23" s="0" t="s">
         <v>139</v>
@@ -3862,22 +3868,22 @@
         <v>212</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>3</v>
+        <v>300</v>
       </c>
       <c r="E24" s="0" t="s">
         <v>213</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>131</v>
+        <v>166</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H24" s="0" t="s">
         <v>139</v>
@@ -3894,8 +3900,7 @@
         <v>0</v>
       </c>
       <c r="D25" s="0" t="n">
-        <f aca="false">PI()</f>
-        <v>3.14159265358979</v>
+        <v>3</v>
       </c>
       <c r="E25" s="0" t="s">
         <v>215</v>
@@ -3904,7 +3909,7 @@
         <v>131</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H25" s="0" t="s">
         <v>139</v>
@@ -3921,7 +3926,8 @@
         <v>0</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>7</v>
+        <f aca="false">PI()</f>
+        <v>3.14159265358979</v>
       </c>
       <c r="E26" s="0" t="s">
         <v>217</v>
@@ -3930,36 +3936,36 @@
         <v>131</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H26" s="0" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="B28" s="0" t="n">
-        <v>36</v>
-      </c>
-      <c r="C28" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="D28" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="E28" s="0" t="s">
+      <c r="B27" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E27" s="0" t="s">
         <v>219</v>
       </c>
-      <c r="F28" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="G28" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="H28" s="0" t="s">
-        <v>152</v>
+      <c r="F27" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3967,22 +3973,22 @@
         <v>220</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>3</v>
+        <v>1000</v>
       </c>
       <c r="E29" s="0" t="s">
         <v>221</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>131</v>
+        <v>159</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H29" s="0" t="s">
         <v>152</v>
@@ -3999,8 +4005,7 @@
         <v>0</v>
       </c>
       <c r="D30" s="0" t="n">
-        <f aca="false">PI()</f>
-        <v>3.14159265358979</v>
+        <v>3</v>
       </c>
       <c r="E30" s="0" t="s">
         <v>223</v>
@@ -4009,7 +4014,7 @@
         <v>131</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H30" s="0" t="s">
         <v>152</v>
@@ -4026,7 +4031,8 @@
         <v>0</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>7</v>
+        <f aca="false">PI()</f>
+        <v>3.14159265358979</v>
       </c>
       <c r="E31" s="0" t="s">
         <v>225</v>
@@ -4035,64 +4041,62 @@
         <v>131</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H31" s="0" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
         <v>226</v>
       </c>
-      <c r="B33" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="C33" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="D33" s="0" t="n">
-        <v>550</v>
-      </c>
-      <c r="E33" s="0" t="s">
+      <c r="B32" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E32" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="F33" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="G33" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="H33" s="0" t="s">
-        <v>228</v>
+      <c r="F32" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="H32" s="0" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>550</v>
+      </c>
+      <c r="E34" s="0" t="s">
         <v>229</v>
       </c>
-      <c r="B34" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="C34" s="0" t="n">
-        <f aca="false">-PI()</f>
-        <v>-3.14159265358979</v>
-      </c>
-      <c r="D34" s="0" t="n">
-        <f aca="false">PI()</f>
-        <v>3.14159265358979</v>
-      </c>
-      <c r="E34" s="0" t="s">
+      <c r="F34" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="H34" s="0" t="s">
         <v>230</v>
-      </c>
-      <c r="F34" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="G34" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="H34" s="0" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4100,13 +4104,15 @@
         <v>231</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C35" s="0" t="n">
-        <v>-2.4</v>
+        <f aca="false">-PI()</f>
+        <v>-3.14159265358979</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>2.4</v>
+        <f aca="false">PI()</f>
+        <v>3.14159265358979</v>
       </c>
       <c r="E35" s="0" t="s">
         <v>232</v>
@@ -4115,10 +4121,10 @@
         <v>131</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4126,25 +4132,25 @@
         <v>233</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>10</v>
+        <v>-2.4</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>300</v>
+        <v>2.4</v>
       </c>
       <c r="E36" s="0" t="s">
         <v>234</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4152,25 +4158,25 @@
         <v>235</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>3</v>
+        <v>300</v>
       </c>
       <c r="E37" s="0" t="s">
         <v>236</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>131</v>
+        <v>166</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4184,8 +4190,7 @@
         <v>0</v>
       </c>
       <c r="D38" s="0" t="n">
-        <f aca="false">PI()</f>
-        <v>3.14159265358979</v>
+        <v>3</v>
       </c>
       <c r="E38" s="0" t="s">
         <v>238</v>
@@ -4194,10 +4199,10 @@
         <v>131</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4211,7 +4216,8 @@
         <v>0</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>7</v>
+        <f aca="false">PI()</f>
+        <v>3.14159265358979</v>
       </c>
       <c r="E39" s="0" t="s">
         <v>240</v>
@@ -4220,10 +4226,36 @@
         <v>131</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="G40" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="H40" s="0" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -4256,7 +4288,7 @@
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.5459183673469"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.7040816326531"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.0918367346939"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -4300,7 +4332,7 @@
         <v>150</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>126</v>
@@ -4406,7 +4438,7 @@
         <v>100</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>126</v>
@@ -4500,7 +4532,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>30</v>
@@ -4512,7 +4544,7 @@
         <v>3</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>131</v>
@@ -4526,7 +4558,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>30</v>
@@ -4539,7 +4571,7 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>131</v>
@@ -4553,7 +4585,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>30</v>
@@ -4565,7 +4597,7 @@
         <v>5</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>131</v>
@@ -4579,7 +4611,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>29</v>
@@ -4591,7 +4623,7 @@
         <v>70</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>183</v>
@@ -4605,7 +4637,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>30</v>
@@ -4617,7 +4649,7 @@
         <v>250</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>166</v>
@@ -4631,7 +4663,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>30</v>
@@ -4643,7 +4675,7 @@
         <v>6</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>131</v>
@@ -4657,7 +4689,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>30</v>
@@ -4671,7 +4703,7 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>131</v>
@@ -4685,7 +4717,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>30</v>
@@ -4697,7 +4729,7 @@
         <v>5</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>131</v>
@@ -4711,7 +4743,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>45</v>
@@ -4723,13 +4755,13 @@
         <v>500</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>166</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H20" s="0" t="s">
         <v>139</v>
@@ -4737,7 +4769,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>30</v>
@@ -4751,13 +4783,13 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>131</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H21" s="0" t="s">
         <v>139</v>
@@ -4765,7 +4797,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>24</v>
@@ -4777,13 +4809,13 @@
         <v>2.4</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>131</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H22" s="0" t="s">
         <v>139</v>
@@ -4791,7 +4823,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>29</v>
@@ -4803,13 +4835,13 @@
         <v>300</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>166</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H23" s="0" t="s">
         <v>139</v>
@@ -4817,7 +4849,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>30</v>
@@ -4829,13 +4861,13 @@
         <v>3</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>131</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H24" s="0" t="s">
         <v>139</v>
@@ -4843,7 +4875,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>30</v>
@@ -4856,13 +4888,13 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>131</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H25" s="0" t="s">
         <v>139</v>
@@ -4870,7 +4902,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>30</v>
@@ -4882,13 +4914,13 @@
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="F26" s="0" t="s">
         <v>131</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H26" s="0" t="s">
         <v>139</v>
@@ -4896,7 +4928,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>45</v>
@@ -4908,13 +4940,13 @@
         <v>1000</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H28" s="0" t="s">
         <v>152</v>
@@ -4922,7 +4954,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>30</v>
@@ -4934,13 +4966,13 @@
         <v>3</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="F29" s="0" t="s">
         <v>131</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H29" s="0" t="s">
         <v>152</v>
@@ -4948,7 +4980,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>30</v>
@@ -4961,13 +4993,13 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="F30" s="0" t="s">
         <v>131</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H30" s="0" t="s">
         <v>152</v>
@@ -4975,7 +5007,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>30</v>
@@ -4987,13 +5019,13 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F31" s="0" t="s">
         <v>131</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H31" s="0" t="s">
         <v>152</v>
@@ -5001,7 +5033,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>25</v>
@@ -5013,21 +5045,21 @@
         <v>550</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="F33" s="0" t="s">
         <v>166</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>30</v>
@@ -5041,21 +5073,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="F34" s="0" t="s">
         <v>131</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>24</v>
@@ -5067,21 +5099,21 @@
         <v>2.4</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="F35" s="0" t="s">
         <v>131</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>29</v>
@@ -5093,21 +5125,21 @@
         <v>300</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="F36" s="0" t="s">
         <v>166</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>30</v>
@@ -5119,21 +5151,21 @@
         <v>3</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="F37" s="0" t="s">
         <v>131</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>30</v>
@@ -5146,21 +5178,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="F38" s="0" t="s">
         <v>131</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>30</v>
@@ -5172,16 +5204,16 @@
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="F39" s="0" t="s">
         <v>131</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -5214,7 +5246,7 @@
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.5459183673469"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.7040816326531"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.0918367346939"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -5364,10 +5396,10 @@
         <v>100</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="G7" s="0" t="s">
         <v>176</v>
@@ -5458,7 +5490,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>30</v>
@@ -5470,7 +5502,7 @@
         <v>3</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>131</v>
@@ -5484,7 +5516,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>30</v>
@@ -5497,7 +5529,7 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>131</v>
@@ -5511,7 +5543,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>30</v>
@@ -5523,7 +5555,7 @@
         <v>5</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>131</v>
@@ -5537,7 +5569,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>30</v>
@@ -5549,7 +5581,7 @@
         <v>200</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>126</v>
@@ -5563,7 +5595,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>30</v>
@@ -5575,7 +5607,7 @@
         <v>250</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>166</v>
@@ -5589,7 +5621,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>30</v>
@@ -5601,7 +5633,7 @@
         <v>6</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>131</v>
@@ -5615,7 +5647,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>30</v>
@@ -5629,7 +5661,7 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>131</v>
@@ -5643,7 +5675,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>30</v>
@@ -5655,7 +5687,7 @@
         <v>5</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>131</v>
@@ -5669,7 +5701,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>45</v>
@@ -5681,13 +5713,13 @@
         <v>500</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>166</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H20" s="0" t="s">
         <v>139</v>
@@ -5695,7 +5727,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>30</v>
@@ -5709,13 +5741,13 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>131</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H21" s="0" t="s">
         <v>139</v>
@@ -5723,7 +5755,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>24</v>
@@ -5735,13 +5767,13 @@
         <v>2.4</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>131</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H22" s="0" t="s">
         <v>139</v>
@@ -5749,7 +5781,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>29</v>
@@ -5761,13 +5793,13 @@
         <v>300</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>166</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H23" s="0" t="s">
         <v>139</v>
@@ -5775,7 +5807,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>30</v>
@@ -5787,13 +5819,13 @@
         <v>3</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>131</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H24" s="0" t="s">
         <v>139</v>
@@ -5801,7 +5833,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>30</v>
@@ -5814,13 +5846,13 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>131</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H25" s="0" t="s">
         <v>139</v>
@@ -5828,7 +5860,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>30</v>
@@ -5840,13 +5872,13 @@
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="F26" s="0" t="s">
         <v>131</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H26" s="0" t="s">
         <v>139</v>
@@ -5854,7 +5886,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>45</v>
@@ -5866,13 +5898,13 @@
         <v>1000</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H28" s="0" t="s">
         <v>152</v>
@@ -5880,7 +5912,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>30</v>
@@ -5892,13 +5924,13 @@
         <v>3</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="F29" s="0" t="s">
         <v>131</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H29" s="0" t="s">
         <v>152</v>
@@ -5906,7 +5938,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>30</v>
@@ -5919,13 +5951,13 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="F30" s="0" t="s">
         <v>131</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H30" s="0" t="s">
         <v>152</v>
@@ -5933,7 +5965,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>30</v>
@@ -5945,13 +5977,13 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="F31" s="0" t="s">
         <v>131</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H31" s="0" t="s">
         <v>152</v>
@@ -5959,7 +5991,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>25</v>
@@ -5971,21 +6003,21 @@
         <v>550</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="F33" s="0" t="s">
         <v>166</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>30</v>
@@ -5999,21 +6031,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="F34" s="0" t="s">
         <v>131</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>24</v>
@@ -6025,21 +6057,21 @@
         <v>2.4</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="F35" s="0" t="s">
         <v>131</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>29</v>
@@ -6051,21 +6083,21 @@
         <v>300</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="F36" s="0" t="s">
         <v>166</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>30</v>
@@ -6077,21 +6109,21 @@
         <v>3</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="F37" s="0" t="s">
         <v>131</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>30</v>
@@ -6104,21 +6136,21 @@
         <v>3.14159265358979</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="F38" s="0" t="s">
         <v>131</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>30</v>
@@ -6130,16 +6162,16 @@
         <v>7</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="F39" s="0" t="s">
         <v>131</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated pileup weighting; and added generators to blt_reader
</commit_message>
<xml_diff>
--- a/data/plotting_lut.xlsx
+++ b/data/plotting_lut.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="datasets_2012" sheetId="1" state="visible" r:id="rId2"/>
@@ -621,13 +621,13 @@
     <t xml:space="preserve">dilepton_mass</t>
   </si>
   <si>
-    <t xml:space="preserve">M_{\mu, \mu} \, [GeV]</t>
+    <t xml:space="preserve">M_{\mu \mu} \, [GeV]</t>
   </si>
   <si>
     <t xml:space="preserve">dilepton_pt</t>
   </si>
   <si>
-    <t xml:space="preserve">p_{T}^{\mu, \mu} \, [GeV]</t>
+    <t xml:space="preserve">p_{T}^{\mu \mu} \, [GeV]</t>
   </si>
   <si>
     <t xml:space="preserve">dilepton_eta</t>
@@ -1098,9 +1098,9 @@
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="B17" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
+      <selection pane="bottomLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1109,7 +1109,7 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1275510204082"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.5255102040816"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6275510204082"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.4183673469388"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
   </cols>
@@ -1953,8 +1953,8 @@
   </sheetPr>
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1963,7 +1963,7 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1275510204082"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.5255102040816"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6275510204082"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.4183673469388"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
   </cols>
@@ -2645,7 +2645,7 @@
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.5459183673469"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.6683673469388"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -3300,8 +3300,8 @@
   </sheetPr>
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3312,7 +3312,7 @@
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.5459183673469"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.6683673469388"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -4322,7 +4322,7 @@
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.5459183673469"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.6683673469388"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -5280,7 +5280,7 @@
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.5459183673469"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.6683673469388"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Updating to run over full 2016 (synchronized!?) data
</commit_message>
<xml_diff>
--- a/data/plotting_lut.xlsx
+++ b/data/plotting_lut.xlsx
@@ -1157,7 +1157,7 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1275510204082"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.9183673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.0204081632653"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.6020408163265"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
   </cols>
@@ -2002,7 +2002,7 @@
   <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C34" activeCellId="0" sqref="C34"/>
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2011,8 +2011,8 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1275510204082"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.9183673469388"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.7091836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.0204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.8112244897959"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -2405,8 +2405,8 @@
         <v>832</v>
       </c>
       <c r="C22" s="0" t="n">
-        <f aca="false">0.32*0.32</f>
-        <v>0.1024</v>
+        <f aca="false">0.32*0.32*1.8</f>
+        <v>0.18432</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>21</v>
@@ -3101,7 +3101,7 @@
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.5459183673469"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="52.9897959183674"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.1785714285714"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -3846,7 +3846,7 @@
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.5459183673469"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="52.9897959183674"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.1785714285714"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -4856,7 +4856,7 @@
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.5459183673469"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="52.9897959183674"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.1785714285714"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -5814,7 +5814,7 @@
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.5459183673469"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3469387755102"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="52.9897959183674"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.1785714285714"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Adding back in JES systematics; new categories working
</commit_message>
<xml_diff>
--- a/data/plotting_lut.xlsx
+++ b/data/plotting_lut.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="datasets_2012" sheetId="1" state="visible" r:id="rId2"/>
@@ -2387,21 +2387,20 @@
   </sheetPr>
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="70.6275510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="81.9693877551021"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.8520408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.0510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="145.469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="65.0102040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="71.8163265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.0255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="63.9336734693878"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="147.948979591837"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="66.0918367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3244,19 +3243,16 @@
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="topLeft" activeCell="A15" activeCellId="1" sqref="B:B A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="94.9285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.96428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.7551020408163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="116.525510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="81.9693877551021"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.96428571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="243.739795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="96.5459183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.6224489795918"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="118.576530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="83.3724489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="248.061224489796"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4554,19 +4550,16 @@
   <dimension ref="A1:H71"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
+      <selection pane="topLeft" activeCell="A24" activeCellId="1" sqref="B:B A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="94.9285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.96428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.7551020408163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="116.525510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="81.9693877551021"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.96428571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="243.739795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="96.5459183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.6224489795918"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="118.576530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="83.3724489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="248.061224489796"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6289,19 +6282,16 @@
   <dimension ref="A1:H93"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="94.9285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.96428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.7551020408163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="116.525510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="81.9693877551021"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.96428571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="243.739795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="96.5459183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.6224489795918"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="118.576530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="83.3724489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="248.061224489796"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8569,19 +8559,18 @@
   </sheetPr>
   <dimension ref="A1:F109"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="1" sqref="B:B C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.6122448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.3571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.7040816326531"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="51.8367346938776"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.3469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.1530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.0255102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3367346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="52.6989795918367"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.780612244898"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="13.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10666,20 +10655,17 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F43" activeCellId="0" sqref="F43"/>
+      <selection pane="bottomLeft" activeCell="F43" activeCellId="1" sqref="B:B F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="94.9285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.96428571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.0714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="116.525510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="81.9693877551021"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.96428571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="243.739795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="96.5459183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.0255102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="118.576530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="83.3724489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="248.061224489796"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11984,19 +11970,16 @@
   <dimension ref="A1:H82"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.5408163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.96428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.7551020408163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="54.6785714285714"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="81.9693877551021"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.96428571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="243.739795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.0969387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.6224489795918"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="55.6173469387755"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="83.3724489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="248.061224489796"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14004,20 +13987,17 @@
   </sheetPr>
   <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F27" activeCellId="1" sqref="B:B F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="94.9285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.96428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="58.530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="81.9693877551021"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.96428571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="243.739795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="96.5459183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.6836734693878"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="59.5051020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="83.3724489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="248.061224489796"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16026,19 +16006,16 @@
   <dimension ref="A1:H81"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="E15" activeCellId="1" sqref="B:B E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="94.9285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.96428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.7551020408163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="116.525510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="81.9693877551021"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.96428571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="243.739795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="96.5459183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.6224489795918"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="118.576530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="83.3724489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="248.061224489796"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18047,19 +18024,16 @@
   <dimension ref="A1:H86"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
+      <selection pane="topLeft" activeCell="D32" activeCellId="1" sqref="B:B D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="94.9285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.96428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.7551020408163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="116.525510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="81.9693877551021"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.96428571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="243.739795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="96.5459183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.6224489795918"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="118.576530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="83.3724489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="248.061224489796"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20172,19 +20146,16 @@
   <dimension ref="A1:H86"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
+      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="94.9285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.96428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="67.7142857142857"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.0510204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.96428571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="243.739795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="96.5459183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.9540816326531"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="68.7908163265306"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.484693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="248.061224489796"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22297,19 +22268,16 @@
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
+      <selection pane="topLeft" activeCell="D34" activeCellId="1" sqref="B:B D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="94.9285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.96428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.7551020408163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="116.525510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="81.9693877551021"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.96428571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="243.739795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="96.5459183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.6224489795918"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="118.576530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="83.3724489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="248.061224489796"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
finishing up for updates
</commit_message>
<xml_diff>
--- a/data/plotting_lut.xlsx
+++ b/data/plotting_lut.xlsx
@@ -756,184 +756,40 @@
     <t xml:space="preserve">ttbar_semilep_fakes</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ttbar_inclusive</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_fakes</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">zjets_m-50_alt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_fakes</t>
-    </r>
+    <t xml:space="preserve">ttbar_inclusive_fakes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zjets_m-50_alt_fakes</t>
   </si>
   <si>
     <t xml:space="preserve">zjets_fakes</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">zjets_m-10to50_alt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_fakes</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">w1jets</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_fakes</t>
-    </r>
+    <t xml:space="preserve">zjets_m-10to50_alt_fakes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w1jets_fakes</t>
   </si>
   <si>
     <t xml:space="preserve">wjets_fakes</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">w2jets</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_fakes</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">w3jets</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_fakes</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">w4jets</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_fakes</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">t_tw</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_fakes</t>
-    </r>
+    <t xml:space="preserve">w2jets_fakes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w3jets_fakes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w4jets_fakes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t_tw_fakes</t>
   </si>
   <si>
     <t xml:space="preserve">t_fakes</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">tbar_tw</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_fakes</t>
-    </r>
+    <t xml:space="preserve">tbar_tw_fakes</t>
   </si>
   <si>
     <t xml:space="preserve">data_prompt</t>
@@ -2485,7 +2341,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2513,11 +2369,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -9452,8 +9303,8 @@
   </sheetPr>
   <dimension ref="A1:F143"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A93" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B120" activeCellId="0" sqref="B120"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A101" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F107" activeCellId="0" sqref="F107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
updates to ttbar systematics, etc.
</commit_message>
<xml_diff>
--- a/data/plotting_lut.xlsx
+++ b/data/plotting_lut.xlsx
@@ -9303,8 +9303,8 @@
   </sheetPr>
   <dimension ref="A1:F143"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A101" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F107" activeCellId="0" sqref="F107"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C47" activeCellId="0" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10107,8 +10107,8 @@
         <v>832</v>
       </c>
       <c r="C45" s="0" t="n">
-        <f aca="false">0.32*0.32</f>
-        <v>0.1024</v>
+        <f aca="false">0.104976</f>
+        <v>0.104976</v>
       </c>
       <c r="D45" s="0" t="s">
         <v>148</v>
@@ -10128,8 +10128,7 @@
         <v>832</v>
       </c>
       <c r="C46" s="0" t="n">
-        <f aca="false">0.32*0.68*2</f>
-        <v>0.4352</v>
+        <v>0.438048</v>
       </c>
       <c r="D46" s="0" t="s">
         <v>150</v>

</xml_diff>

<commit_message>
Fixed bug in top pt templates
</commit_message>
<xml_diff>
--- a/data/plotting_lut.xlsx
+++ b/data/plotting_lut.xlsx
@@ -9313,7 +9313,7 @@
   <dimension ref="A1:F144"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A36" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D62" activeCellId="0" sqref="D62"/>
+      <selection pane="topLeft" activeCell="C74" activeCellId="0" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10617,8 +10617,7 @@
         <v>4757</v>
       </c>
       <c r="C71" s="0" t="n">
-        <f aca="false">$B$69/SUM($B$71:$B$73)</f>
-        <v>0.963998461615638</v>
+        <v>1</v>
       </c>
       <c r="D71" s="0" t="s">
         <v>190</v>
@@ -10638,8 +10637,7 @@
         <v>884.4</v>
       </c>
       <c r="C72" s="0" t="n">
-        <f aca="false">$B$69/SUM($B$71:$B$73)</f>
-        <v>0.963998461615638</v>
+        <v>1</v>
       </c>
       <c r="D72" s="0" t="s">
         <v>190</v>
@@ -10659,8 +10657,7 @@
         <v>338.9</v>
       </c>
       <c r="C73" s="0" t="n">
-        <f aca="false">$B$69/SUM($B$71:$B$73)</f>
-        <v>0.963998461615638</v>
+        <v>0.95</v>
       </c>
       <c r="D73" s="0" t="s">
         <v>190</v>

</xml_diff>

<commit_message>
partial unblinding a go-go
</commit_message>
<xml_diff>
--- a/data/plotting_lut.xlsx
+++ b/data/plotting_lut.xlsx
@@ -9310,7 +9310,7 @@
   <dimension ref="A1:F144"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F56" activeCellId="0" sqref="F56"/>
+      <selection pane="topLeft" activeCell="J48" activeCellId="0" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9909,10 +9909,10 @@
         <v>137</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>1.1</v>
+        <v>1</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>7</v>
@@ -9929,10 +9929,10 @@
         <v>138</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>1.1</v>
+        <v>1</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>7</v>
@@ -9949,10 +9949,10 @@
         <v>139</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="C35" s="0" t="n">
-        <v>1.1</v>
+        <v>1</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>7</v>
@@ -9969,10 +9969,10 @@
         <v>140</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>1.1</v>
+        <v>1</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>7</v>
@@ -9989,10 +9989,10 @@
         <v>141</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>1.1</v>
+        <v>1</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>7</v>
@@ -10009,10 +10009,10 @@
         <v>142</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="C38" s="0" t="n">
-        <v>1.1</v>
+        <v>1</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>7</v>
@@ -10029,10 +10029,10 @@
         <v>143</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="C39" s="0" t="n">
-        <v>1.1</v>
+        <v>1</v>
       </c>
       <c r="D39" s="0" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Investigating JES and electron related systematics
</commit_message>
<xml_diff>
--- a/data/plotting_lut.xlsx
+++ b/data/plotting_lut.xlsx
@@ -9312,8 +9312,8 @@
   </sheetPr>
   <dimension ref="A1:F144"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A100" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D137" activeCellId="0" sqref="D137"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C77" activeCellId="0" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10617,7 +10617,7 @@
         <v>4757</v>
       </c>
       <c r="C71" s="0" t="n">
-        <v>0.95</v>
+        <v>0.97</v>
       </c>
       <c r="D71" s="0" t="s">
         <v>189</v>
@@ -10637,7 +10637,7 @@
         <v>884.4</v>
       </c>
       <c r="C72" s="0" t="n">
-        <v>0.95</v>
+        <v>0.96</v>
       </c>
       <c r="D72" s="0" t="s">
         <v>189</v>
@@ -10657,7 +10657,7 @@
         <v>338.9</v>
       </c>
       <c r="C73" s="0" t="n">
-        <v>0.95</v>
+        <v>1.005</v>
       </c>
       <c r="D73" s="0" t="s">
         <v>189</v>

</xml_diff>

<commit_message>
uncommented bb_penalty_jac (this should have been included :\)
</commit_message>
<xml_diff>
--- a/data/plotting_lut.xlsx
+++ b/data/plotting_lut.xlsx
@@ -2533,7 +2533,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="B2" activeCellId="1" sqref="C84:C87 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3387,7 +3387,7 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
+      <selection pane="topLeft" activeCell="I9" activeCellId="1" sqref="C84:C87 I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4844,7 +4844,7 @@
   <dimension ref="A1:I71"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
+      <selection pane="topLeft" activeCell="J7" activeCellId="1" sqref="C84:C87 J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6774,7 +6774,7 @@
   <dimension ref="A1:I93"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L34" activeCellId="0" sqref="L34"/>
+      <selection pane="topLeft" activeCell="L34" activeCellId="1" sqref="C84:C87 L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9313,7 +9313,7 @@
   <dimension ref="A1:F144"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C77" activeCellId="0" sqref="C77"/>
+      <selection pane="topLeft" activeCell="C84" activeCellId="0" sqref="C84:C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10886,7 +10886,7 @@
         <v>11486.53</v>
       </c>
       <c r="C84" s="0" t="n">
-        <v>1</v>
+        <v>1.1</v>
       </c>
       <c r="D84" s="0" t="s">
         <v>21</v>
@@ -10907,7 +10907,7 @@
         <v>3775.2</v>
       </c>
       <c r="C85" s="0" t="n">
-        <v>1</v>
+        <v>1.1</v>
       </c>
       <c r="D85" s="0" t="s">
         <v>21</v>
@@ -10928,7 +10928,7 @@
         <v>1139.82</v>
       </c>
       <c r="C86" s="0" t="n">
-        <v>1</v>
+        <v>1.1</v>
       </c>
       <c r="D86" s="0" t="s">
         <v>21</v>
@@ -10949,7 +10949,7 @@
         <v>655.82</v>
       </c>
       <c r="C87" s="0" t="n">
-        <v>1</v>
+        <v>1.1</v>
       </c>
       <c r="D87" s="0" t="s">
         <v>21</v>
@@ -12070,7 +12070,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D66" activeCellId="0" sqref="D66"/>
+      <selection pane="bottomLeft" activeCell="D66" activeCellId="1" sqref="C84:C87 D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13535,7 +13535,7 @@
   <dimension ref="A1:I82"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J71" activeCellId="0" sqref="J71"/>
+      <selection pane="topLeft" activeCell="J71" activeCellId="1" sqref="C84:C87 J71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15784,7 +15784,7 @@
   <dimension ref="A1:I82"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I50" activeCellId="0" sqref="I50"/>
+      <selection pane="topLeft" activeCell="I50" activeCellId="1" sqref="C84:C87 I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18033,7 +18033,7 @@
   <dimension ref="A1:I81"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O80" activeCellId="0" sqref="O80"/>
+      <selection pane="topLeft" activeCell="O80" activeCellId="1" sqref="C84:C87 O80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20282,7 +20282,7 @@
   <dimension ref="A1:I86"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J44" activeCellId="0" sqref="J44"/>
+      <selection pane="topLeft" activeCell="J44" activeCellId="1" sqref="C84:C87 J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22652,7 +22652,7 @@
   <dimension ref="A1:I86"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+      <selection pane="topLeft" activeCell="I4" activeCellId="1" sqref="C84:C87 I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -25017,7 +25017,7 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="1" sqref="C84:C87 I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Adding in fake validation notebook (should have already been done...)
</commit_message>
<xml_diff>
--- a/data/plotting_lut.xlsx
+++ b/data/plotting_lut.xlsx
@@ -2533,7 +2533,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B2" activeCellId="1" sqref="C84:C87 B2"/>
+      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3387,7 +3387,7 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I9" activeCellId="1" sqref="C84:C87 I9"/>
+      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4844,7 +4844,7 @@
   <dimension ref="A1:I71"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J7" activeCellId="1" sqref="C84:C87 J7"/>
+      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6774,7 +6774,7 @@
   <dimension ref="A1:I93"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L34" activeCellId="1" sqref="C84:C87 L34"/>
+      <selection pane="topLeft" activeCell="L34" activeCellId="0" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9312,8 +9312,8 @@
   </sheetPr>
   <dimension ref="A1:F144"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C84" activeCellId="0" sqref="C84:C87"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A94" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B120" activeCellId="0" sqref="B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12070,7 +12070,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D66" activeCellId="1" sqref="C84:C87 D66"/>
+      <selection pane="bottomLeft" activeCell="D66" activeCellId="0" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13535,7 +13535,7 @@
   <dimension ref="A1:I82"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J71" activeCellId="1" sqref="C84:C87 J71"/>
+      <selection pane="topLeft" activeCell="J71" activeCellId="0" sqref="J71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15784,7 +15784,7 @@
   <dimension ref="A1:I82"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I50" activeCellId="1" sqref="C84:C87 I50"/>
+      <selection pane="topLeft" activeCell="I50" activeCellId="0" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18033,7 +18033,7 @@
   <dimension ref="A1:I81"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O80" activeCellId="1" sqref="C84:C87 O80"/>
+      <selection pane="topLeft" activeCell="O80" activeCellId="0" sqref="O80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20282,7 +20282,7 @@
   <dimension ref="A1:I86"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J44" activeCellId="1" sqref="C84:C87 J44"/>
+      <selection pane="topLeft" activeCell="J44" activeCellId="0" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22652,7 +22652,7 @@
   <dimension ref="A1:I86"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="1" sqref="C84:C87 I4"/>
+      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -25017,7 +25017,7 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="1" sqref="C84:C87 I2"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Working on results plots
</commit_message>
<xml_diff>
--- a/data/plotting_lut.xlsx
+++ b/data/plotting_lut.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="datasets_2012" sheetId="1" state="visible" r:id="rId2"/>
@@ -2652,7 +2652,7 @@
       <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="71.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.03"/>
@@ -3501,13 +3501,13 @@
   </sheetPr>
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="96.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="51.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="118.6"/>
@@ -4961,7 +4961,7 @@
       <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="96.57"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="3" min="2" style="0" width="8.67"/>
@@ -6890,7 +6890,7 @@
       <selection pane="topLeft" activeCell="L34" activeCellId="0" sqref="L34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="96.57"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="3" min="2" style="0" width="8.67"/>
@@ -9424,11 +9424,11 @@
   </sheetPr>
   <dimension ref="A1:F168"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A115" activeCellId="0" sqref="A115"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A50" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C74" activeCellId="0" sqref="C74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.68"/>
@@ -10685,7 +10685,7 @@
         <v>190</v>
       </c>
       <c r="B68" s="0" t="n">
-        <v>4757</v>
+        <v>5330</v>
       </c>
       <c r="C68" s="0" t="n">
         <v>0.97</v>
@@ -10705,7 +10705,7 @@
         <v>192</v>
       </c>
       <c r="B69" s="0" t="n">
-        <v>884.4</v>
+        <v>966.5</v>
       </c>
       <c r="C69" s="0" t="n">
         <v>0.96</v>
@@ -10725,7 +10725,7 @@
         <v>194</v>
       </c>
       <c r="B70" s="0" t="n">
-        <v>338.9</v>
+        <v>359.3</v>
       </c>
       <c r="C70" s="0" t="n">
         <v>1.005</v>
@@ -11113,8 +11113,7 @@
         <v>217</v>
       </c>
       <c r="B89" s="0" t="n">
-        <f aca="false">9493*1.21</f>
-        <v>11486.53</v>
+        <v>9622</v>
       </c>
       <c r="C89" s="0" t="n">
         <v>1</v>
@@ -11134,8 +11133,7 @@
         <v>220</v>
       </c>
       <c r="B90" s="0" t="n">
-        <f aca="false">3120*1.21</f>
-        <v>3775.2</v>
+        <v>3149</v>
       </c>
       <c r="C90" s="0" t="n">
         <v>1</v>
@@ -11155,8 +11153,7 @@
         <v>222</v>
       </c>
       <c r="B91" s="0" t="n">
-        <f aca="false">942*1.21</f>
-        <v>1139.82</v>
+        <v>948.1</v>
       </c>
       <c r="C91" s="0" t="n">
         <v>1</v>
@@ -11176,8 +11173,7 @@
         <v>224</v>
       </c>
       <c r="B92" s="0" t="n">
-        <f aca="false">542*1.21</f>
-        <v>655.82</v>
+        <v>495.1</v>
       </c>
       <c r="C92" s="0" t="n">
         <v>1</v>
@@ -12687,7 +12683,7 @@
       <selection pane="bottomLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.03"/>
@@ -14149,7 +14145,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="51.62"/>
@@ -16453,7 +16449,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.68"/>
@@ -18757,7 +18753,7 @@
       <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.47"/>
@@ -21061,7 +21057,7 @@
       <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="96.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="51.62"/>
@@ -23428,7 +23424,7 @@
       <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.94"/>
@@ -25790,7 +25786,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="96.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="8.67"/>

</xml_diff>